<commit_message>
updated TPCs for immune genes to show models for all 3 treatments on one fig
</commit_message>
<xml_diff>
--- a/Gene_temp_data.xlsx
+++ b/Gene_temp_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linzm\Documents\Tate Lab Rotation\Tate_Rotation_Temp_Immunity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F200F37C-B40E-46F9-B28C-86460D945615}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DCA4CF-38E1-406A-9E81-C4CF2ACD4E1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="4" xr2:uid="{B3C2EB18-1E1E-4520-B7BE-6EC39DD43585}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="5" xr2:uid="{B3C2EB18-1E1E-4520-B7BE-6EC39DD43585}"/>
   </bookViews>
   <sheets>
     <sheet name="Relish" sheetId="14" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="BtMid" sheetId="15" r:id="rId3"/>
     <sheet name="IMD" sheetId="16" r:id="rId4"/>
     <sheet name="Gene_Data" sheetId="17" r:id="rId5"/>
+    <sheet name="BtMid_GeneData" sheetId="18" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Gene_Data!$C$1:$C$163</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="192">
   <si>
     <t>Well Position</t>
   </si>
@@ -7918,7 +7919,7 @@
   <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -11841,11 +11842,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F70D3E-EA3F-4D40-9E3D-2763A8ADCA53}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:D163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L68" sqref="L68"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -11870,7 +11870,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>24</v>
       </c>
@@ -11884,7 +11884,7 @@
         <v>1.4968999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>24</v>
       </c>
@@ -11898,7 +11898,7 @@
         <v>4.4233000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>24</v>
       </c>
@@ -11912,7 +11912,7 @@
         <v>51.712000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>24</v>
       </c>
@@ -11926,7 +11926,7 @@
         <v>1.2423</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>24</v>
       </c>
@@ -11940,7 +11940,7 @@
         <v>4.2953999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>24</v>
       </c>
@@ -11954,7 +11954,7 @@
         <v>20.6371</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>24</v>
       </c>
@@ -11968,7 +11968,7 @@
         <v>1.1293</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>24</v>
       </c>
@@ -11982,7 +11982,7 @@
         <v>2.4594</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>24</v>
       </c>
@@ -11996,7 +11996,7 @@
         <v>44.673900000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>24</v>
       </c>
@@ -12010,7 +12010,7 @@
         <v>1.2533000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>24</v>
       </c>
@@ -12024,7 +12024,7 @@
         <v>13.443899999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>24</v>
       </c>
@@ -12038,7 +12038,7 @@
         <v>32.5351</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>24</v>
       </c>
@@ -12052,7 +12052,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A15">
         <v>24</v>
       </c>
@@ -12066,7 +12066,7 @@
         <v>2.9918</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A16">
         <v>24</v>
       </c>
@@ -12080,7 +12080,7 @@
         <v>17.4602</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A17">
         <v>24</v>
       </c>
@@ -12094,7 +12094,7 @@
         <v>0.61080000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A18">
         <v>24</v>
       </c>
@@ -12108,7 +12108,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A19">
         <v>24</v>
       </c>
@@ -12122,7 +12122,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A20">
         <v>30</v>
       </c>
@@ -12136,7 +12136,7 @@
         <v>11.2843</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A21">
         <v>30</v>
       </c>
@@ -12150,7 +12150,7 @@
         <v>2.3896000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A22">
         <v>30</v>
       </c>
@@ -12164,7 +12164,7 @@
         <v>0.75360000000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A23">
         <v>30</v>
       </c>
@@ -12178,7 +12178,7 @@
         <v>8.2329000000000008</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A24">
         <v>30</v>
       </c>
@@ -12192,7 +12192,7 @@
         <v>4.6044999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A25">
         <v>30</v>
       </c>
@@ -12206,7 +12206,7 @@
         <v>0.79220000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A26">
         <v>30</v>
       </c>
@@ -12220,7 +12220,7 @@
         <v>11.7745</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A27">
         <v>30</v>
       </c>
@@ -12234,7 +12234,7 @@
         <v>8.2761999999999993</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A28">
         <v>30</v>
       </c>
@@ -12248,7 +12248,7 @@
         <v>0.32969999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A29">
         <v>30</v>
       </c>
@@ -12262,7 +12262,7 @@
         <v>6.7778999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A30">
         <v>30</v>
       </c>
@@ -12276,7 +12276,7 @@
         <v>3.2662</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A31">
         <v>30</v>
       </c>
@@ -12290,7 +12290,7 @@
         <v>1.1875</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A32">
         <v>30</v>
       </c>
@@ -12304,7 +12304,7 @@
         <v>27.4818</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A33">
         <v>30</v>
       </c>
@@ -12318,7 +12318,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A34">
         <v>30</v>
       </c>
@@ -12332,7 +12332,7 @@
         <v>2.5034999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A35">
         <v>30</v>
       </c>
@@ -12346,7 +12346,7 @@
         <v>0.62280000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A36">
         <v>30</v>
       </c>
@@ -12360,7 +12360,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A37">
         <v>30</v>
       </c>
@@ -12374,7 +12374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A38">
         <v>34</v>
       </c>
@@ -12388,7 +12388,7 @@
         <v>1.4032</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A39">
         <v>34</v>
       </c>
@@ -12402,7 +12402,7 @@
         <v>0.84630000000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A40">
         <v>34</v>
       </c>
@@ -12416,7 +12416,7 @@
         <v>22.253799999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A41">
         <v>34</v>
       </c>
@@ -12430,7 +12430,7 @@
         <v>1.9323999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A42">
         <v>34</v>
       </c>
@@ -12444,7 +12444,7 @@
         <v>2.8921000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A43">
         <v>34</v>
       </c>
@@ -12458,7 +12458,7 @@
         <v>11.955500000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A44">
         <v>34</v>
       </c>
@@ -12472,7 +12472,7 @@
         <v>0.91059999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A45">
         <v>34</v>
       </c>
@@ -12486,7 +12486,7 @@
         <v>2.4357000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A46">
         <v>34</v>
       </c>
@@ -12500,7 +12500,7 @@
         <v>10.7469</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A47">
         <v>34</v>
       </c>
@@ -12514,7 +12514,7 @@
         <v>2.6364000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A48">
         <v>34</v>
       </c>
@@ -12528,7 +12528,7 @@
         <v>2.3853</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A49">
         <v>34</v>
       </c>
@@ -12542,7 +12542,7 @@
         <v>6.4763999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A50">
         <v>34</v>
       </c>
@@ -12556,7 +12556,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A51">
         <v>34</v>
       </c>
@@ -12570,7 +12570,7 @@
         <v>4.8316999999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A52">
         <v>34</v>
       </c>
@@ -12584,7 +12584,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A53">
         <v>34</v>
       </c>
@@ -12598,7 +12598,7 @@
         <v>1.0620000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A54">
         <v>34</v>
       </c>
@@ -12612,7 +12612,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A55">
         <v>34</v>
       </c>
@@ -13382,7 +13382,7 @@
         <v>0.98444900580502814</v>
       </c>
     </row>
-    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A110">
         <v>24</v>
       </c>
@@ -13396,7 +13396,7 @@
         <v>2.1242971520355334</v>
       </c>
     </row>
-    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A111">
         <v>24</v>
       </c>
@@ -13410,7 +13410,7 @@
         <v>4.291706844760796</v>
       </c>
     </row>
-    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A112">
         <v>24</v>
       </c>
@@ -13424,7 +13424,7 @@
         <v>4.0973316061281428</v>
       </c>
     </row>
-    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A113">
         <v>24</v>
       </c>
@@ -13438,7 +13438,7 @@
         <v>1.4003082825932121</v>
       </c>
     </row>
-    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A114">
         <v>24</v>
       </c>
@@ -13452,7 +13452,7 @@
         <v>4.2822781418585629</v>
       </c>
     </row>
-    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A115">
         <v>24</v>
       </c>
@@ -13466,7 +13466,7 @@
         <v>24.879857304108231</v>
       </c>
     </row>
-    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A116">
         <v>24</v>
       </c>
@@ -13480,7 +13480,7 @@
         <v>2.1361512628337644</v>
       </c>
     </row>
-    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A117">
         <v>24</v>
       </c>
@@ -13494,7 +13494,7 @@
         <v>4.4234725395964745</v>
       </c>
     </row>
-    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A118">
         <v>24</v>
       </c>
@@ -13508,7 +13508,7 @@
         <v>24.233747546798313</v>
       </c>
     </row>
-    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A119">
         <v>24</v>
       </c>
@@ -13522,7 +13522,7 @@
         <v>2.4320009352248682</v>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A120">
         <v>24</v>
       </c>
@@ -13536,7 +13536,7 @@
         <v>3.2087767766407076</v>
       </c>
     </row>
-    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A121">
         <v>24</v>
       </c>
@@ -13550,7 +13550,7 @@
         <v>11.923025326389997</v>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A122">
         <v>24</v>
       </c>
@@ -13564,7 +13564,7 @@
         <v>4.0303255151733959</v>
       </c>
     </row>
-    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A123">
         <v>24</v>
       </c>
@@ -13578,7 +13578,7 @@
         <v>5.4793397531315007</v>
       </c>
     </row>
-    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A124">
         <v>24</v>
       </c>
@@ -13592,7 +13592,7 @@
         <v>3.8660381950190703</v>
       </c>
     </row>
-    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A125">
         <v>24</v>
       </c>
@@ -13606,7 +13606,7 @@
         <v>0.78798330374844805</v>
       </c>
     </row>
-    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A126">
         <v>24</v>
       </c>
@@ -13620,7 +13620,7 @@
         <v>4.1156288923036524</v>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A127">
         <v>24</v>
       </c>
@@ -13634,7 +13634,7 @@
         <v>17.584575159373117</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A128">
         <v>30</v>
       </c>
@@ -13648,7 +13648,7 @@
         <v>0.62926575287712383</v>
       </c>
     </row>
-    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A129">
         <v>30</v>
       </c>
@@ -13662,7 +13662,7 @@
         <v>1.4813329696016226</v>
       </c>
     </row>
-    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A130">
         <v>30</v>
       </c>
@@ -13676,7 +13676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A131">
         <v>30</v>
       </c>
@@ -13690,7 +13690,7 @@
         <v>8.4712330715386397</v>
       </c>
     </row>
-    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A132">
         <v>30</v>
       </c>
@@ -13704,7 +13704,7 @@
         <v>2.193379100598857</v>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A133">
         <v>30</v>
       </c>
@@ -13718,7 +13718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A134">
         <v>30</v>
       </c>
@@ -13732,7 +13732,7 @@
         <v>7.2401684522156904</v>
       </c>
     </row>
-    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A135">
         <v>30</v>
       </c>
@@ -13746,7 +13746,7 @@
         <v>2.8798616356860864</v>
       </c>
     </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A136">
         <v>30</v>
       </c>
@@ -13760,7 +13760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A137">
         <v>30</v>
       </c>
@@ -13774,7 +13774,7 @@
         <v>4.9186883858404551</v>
       </c>
     </row>
-    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A138">
         <v>30</v>
       </c>
@@ -13788,7 +13788,7 @@
         <v>2.4557101522683311</v>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A139">
         <v>30</v>
       </c>
@@ -13802,7 +13802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A140">
         <v>30</v>
       </c>
@@ -13816,7 +13816,7 @@
         <v>6.6619319408771291</v>
       </c>
     </row>
-    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A141">
         <v>30</v>
       </c>
@@ -13830,7 +13830,7 @@
         <v>1.1542815525474373</v>
       </c>
     </row>
-    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A142">
         <v>30</v>
       </c>
@@ -13844,7 +13844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A143">
         <v>30</v>
       </c>
@@ -13858,7 +13858,7 @@
         <v>1.549177517412722</v>
       </c>
     </row>
-    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A144">
         <v>30</v>
       </c>
@@ -13872,7 +13872,7 @@
         <v>1.1568740304497094</v>
       </c>
     </row>
-    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A145">
         <v>30</v>
       </c>
@@ -13886,7 +13886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A146">
         <v>34</v>
       </c>
@@ -13900,7 +13900,7 @@
         <v>0.99202811345468989</v>
       </c>
     </row>
-    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A147">
         <v>34</v>
       </c>
@@ -13914,7 +13914,7 @@
         <v>2.9354500638805625</v>
       </c>
     </row>
-    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A148">
         <v>34</v>
       </c>
@@ -13928,7 +13928,7 @@
         <v>24.403576764692222</v>
       </c>
     </row>
-    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A149">
         <v>34</v>
       </c>
@@ -13942,7 +13942,7 @@
         <v>1.1534283003134</v>
       </c>
     </row>
-    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A150">
         <v>34</v>
       </c>
@@ -13956,7 +13956,7 @@
         <v>1.6447935076908315</v>
       </c>
     </row>
-    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A151">
         <v>34</v>
       </c>
@@ -13970,7 +13970,7 @@
         <v>12.04132253526303</v>
       </c>
     </row>
-    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A152">
         <v>34</v>
       </c>
@@ -13984,7 +13984,7 @@
         <v>1.4431478418462336</v>
       </c>
     </row>
-    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A153">
         <v>34</v>
       </c>
@@ -13998,7 +13998,7 @@
         <v>1.9697043994046894</v>
       </c>
     </row>
-    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A154">
         <v>34</v>
       </c>
@@ -14012,7 +14012,7 @@
         <v>8.0077394567386389</v>
       </c>
     </row>
-    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A155">
         <v>34</v>
       </c>
@@ -14026,7 +14026,7 @@
         <v>0.73189952870282604</v>
       </c>
     </row>
-    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A156">
         <v>34</v>
       </c>
@@ -14040,7 +14040,7 @@
         <v>2.2680177969894908</v>
       </c>
     </row>
-    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A157">
         <v>34</v>
       </c>
@@ -14054,7 +14054,7 @@
         <v>2.6709889194904322</v>
       </c>
     </row>
-    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A158">
         <v>34</v>
       </c>
@@ -14068,7 +14068,7 @@
         <v>0.65358061447701277</v>
       </c>
     </row>
-    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A159">
         <v>34</v>
       </c>
@@ -14082,7 +14082,7 @@
         <v>1.2592706200551125</v>
       </c>
     </row>
-    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A160">
         <v>34</v>
       </c>
@@ -14096,7 +14096,7 @@
         <v>2.6209052397289865</v>
       </c>
     </row>
-    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A161">
         <v>34</v>
       </c>
@@ -14110,7 +14110,7 @@
         <v>0.59701234632890421</v>
       </c>
     </row>
-    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A162">
         <v>34</v>
       </c>
@@ -14124,7 +14124,7 @@
         <v>0.34434875232192103</v>
       </c>
     </row>
-    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.75">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A163">
         <v>34</v>
       </c>
@@ -14139,13 +14139,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C163" xr:uid="{33A90D7F-BF7B-477D-AF5A-1703D07EDBD8}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Cactus"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="C1:C163" xr:uid="{33A90D7F-BF7B-477D-AF5A-1703D07EDBD8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A56:D109">
     <sortCondition ref="B2:B163"/>
   </sortState>
@@ -14154,13 +14148,795 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4ADEF0-7664-4391-A09C-F24CBB51FD97}">
+  <dimension ref="A1:D55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="7.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2">
+        <v>8.07</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4">
+        <v>55.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5">
+        <v>4.33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6">
+        <v>4.42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7">
+        <v>237.44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A8">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A9">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10">
+        <v>25.26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A11">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A12">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12">
+        <v>3.47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A13">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A14">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A15">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A16">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16">
+        <v>11.24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A17">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A18">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A19">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D19">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A20">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" t="s">
+        <v>186</v>
+      </c>
+      <c r="D20">
+        <v>129.44999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A21">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" t="s">
+        <v>186</v>
+      </c>
+      <c r="D21">
+        <v>20.64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A23">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23">
+        <v>415.91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A24">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24">
+        <v>31.69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A25">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A26">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" t="s">
+        <v>186</v>
+      </c>
+      <c r="D26">
+        <v>81.86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A27">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>180</v>
+      </c>
+      <c r="C27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D27">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A28">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>179</v>
+      </c>
+      <c r="C28" t="s">
+        <v>186</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A29">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>181</v>
+      </c>
+      <c r="C29" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29">
+        <v>207.56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>180</v>
+      </c>
+      <c r="C30" t="s">
+        <v>186</v>
+      </c>
+      <c r="D30">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" t="s">
+        <v>186</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>181</v>
+      </c>
+      <c r="C32" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32">
+        <v>17.93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>180</v>
+      </c>
+      <c r="C33" t="s">
+        <v>186</v>
+      </c>
+      <c r="D33">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>179</v>
+      </c>
+      <c r="C34" t="s">
+        <v>186</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>181</v>
+      </c>
+      <c r="C35" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35">
+        <v>19.239999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A36">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>180</v>
+      </c>
+      <c r="C36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A37">
+        <v>30</v>
+      </c>
+      <c r="B37" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" t="s">
+        <v>186</v>
+      </c>
+      <c r="D38">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A39">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39">
+        <v>50.15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A40">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>181</v>
+      </c>
+      <c r="C40" t="s">
+        <v>186</v>
+      </c>
+      <c r="D40">
+        <v>1733.65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A41">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41" t="s">
+        <v>186</v>
+      </c>
+      <c r="D41">
+        <v>3.19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A42">
+        <v>34</v>
+      </c>
+      <c r="B42" t="s">
+        <v>180</v>
+      </c>
+      <c r="C42" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A43">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C43" t="s">
+        <v>186</v>
+      </c>
+      <c r="D43">
+        <v>180.58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A44">
+        <v>34</v>
+      </c>
+      <c r="B44" t="s">
+        <v>179</v>
+      </c>
+      <c r="C44" t="s">
+        <v>186</v>
+      </c>
+      <c r="D44">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A45">
+        <v>34</v>
+      </c>
+      <c r="B45" t="s">
+        <v>180</v>
+      </c>
+      <c r="C45" t="s">
+        <v>186</v>
+      </c>
+      <c r="D45">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A46">
+        <v>34</v>
+      </c>
+      <c r="B46" t="s">
+        <v>181</v>
+      </c>
+      <c r="C46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D46">
+        <v>176.34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A47">
+        <v>34</v>
+      </c>
+      <c r="B47" t="s">
+        <v>179</v>
+      </c>
+      <c r="C47" t="s">
+        <v>186</v>
+      </c>
+      <c r="D47">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A48">
+        <v>34</v>
+      </c>
+      <c r="B48" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" t="s">
+        <v>186</v>
+      </c>
+      <c r="D48">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A49">
+        <v>34</v>
+      </c>
+      <c r="B49" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" t="s">
+        <v>186</v>
+      </c>
+      <c r="D49">
+        <v>315.66000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A50">
+        <v>34</v>
+      </c>
+      <c r="B50" t="s">
+        <v>179</v>
+      </c>
+      <c r="C50" t="s">
+        <v>186</v>
+      </c>
+      <c r="D50">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A51">
+        <v>34</v>
+      </c>
+      <c r="B51" t="s">
+        <v>180</v>
+      </c>
+      <c r="C51" t="s">
+        <v>186</v>
+      </c>
+      <c r="D51">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A52">
+        <v>34</v>
+      </c>
+      <c r="B52" t="s">
+        <v>181</v>
+      </c>
+      <c r="C52" t="s">
+        <v>186</v>
+      </c>
+      <c r="D52">
+        <v>22.75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A53">
+        <v>34</v>
+      </c>
+      <c r="B53" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" t="s">
+        <v>186</v>
+      </c>
+      <c r="D53">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A54">
+        <v>34</v>
+      </c>
+      <c r="B54" t="s">
+        <v>180</v>
+      </c>
+      <c r="C54" t="s">
+        <v>186</v>
+      </c>
+      <c r="D54">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A55">
+        <v>34</v>
+      </c>
+      <c r="B55" t="s">
+        <v>181</v>
+      </c>
+      <c r="C55" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55">
+        <v>9.9600000000000009</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5AAFFED5B596D4BAE4CE19A95039785" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb12f4776e238e1f586e33791f07bb77">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d40adf4f-7ef1-43d3-876d-177d4150ba93" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fdb1f1d4a4ea75ce4d5cd3fd2a25377c" ns3:_="">
     <xsd:import namespace="d40adf4f-7ef1-43d3-876d-177d4150ba93"/>
@@ -14324,6 +15100,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -14334,22 +15116,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6078DB98-64DD-44CA-A39B-9F3CF9F2C375}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d40adf4f-7ef1-43d3-876d-177d4150ba93"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29811117-64F0-425E-BDF0-8D1838742348}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14367,6 +15133,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6078DB98-64DD-44CA-A39B-9F3CF9F2C375}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d40adf4f-7ef1-43d3-876d-177d4150ba93"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34B288BE-7AE7-404E-A200-18C81F874FA2}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
updates to ODEs, figuring out equations and graphing
</commit_message>
<xml_diff>
--- a/Gene_temp_data.xlsx
+++ b/Gene_temp_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linzm\Documents\Tate Lab Rotation\Tate_Rotation_Temp_Immunity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DCA4CF-38E1-406A-9E81-C4CF2ACD4E1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E4A814-3FDB-4ED2-B15D-AD1BAEE84198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="5" xr2:uid="{B3C2EB18-1E1E-4520-B7BE-6EC39DD43585}"/>
   </bookViews>
@@ -11845,7 +11845,7 @@
   <dimension ref="A1:D163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>

</xml_diff>

<commit_message>
new changes to TPCs, Flinn model is best for immune genes; Changes to ODEs based on 11/2 workshop presentation
</commit_message>
<xml_diff>
--- a/Gene_temp_data.xlsx
+++ b/Gene_temp_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linzm\Documents\Tate Lab Rotation\Tate_Rotation_Temp_Immunity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E4A814-3FDB-4ED2-B15D-AD1BAEE84198}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBEEEAD-D4C1-4286-B3D2-BAFD971FF031}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="5" xr2:uid="{B3C2EB18-1E1E-4520-B7BE-6EC39DD43585}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" firstSheet="1" activeTab="6" xr2:uid="{B3C2EB18-1E1E-4520-B7BE-6EC39DD43585}"/>
   </bookViews>
   <sheets>
     <sheet name="Relish" sheetId="14" r:id="rId1"/>
@@ -19,9 +19,11 @@
     <sheet name="IMD" sheetId="16" r:id="rId4"/>
     <sheet name="Gene_Data" sheetId="17" r:id="rId5"/>
     <sheet name="BtMid_GeneData" sheetId="18" r:id="rId6"/>
+    <sheet name="Gene_Data_Modified" sheetId="19" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Gene_Data!$C$1:$C$163</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Gene_Data_Modified!$B$1:$B$205</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">(Cactus!$F$2,Cactus!$F$5,Cactus!$F$8,Cactus!$F$11,Cactus!$F$14,Cactus!$F$17,Cactus!$F$22,Cactus!$F$25,Cactus!$F$28,Cactus!$F$31,Cactus!$F$34,Cactus!$F$37,Cactus!$F$38,Cactus!$F$41,Cactus!$F$44,Cactus!$F$47,Cactus!$F$50,Cactus!$F$54,Cactus!$F$53)</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">(Cactus!$F$3,Cactus!$F$6,Cactus!$F$9,Cactus!$F$12,Cactus!$F$15,Cactus!$F$18,Cactus!$F$21,Cactus!$F$24,Cactus!$F$27,Cactus!$F$30,Cactus!$F$33,Cactus!$F$36,Cactus!$F$39,Cactus!$F$42,Cactus!$F$45,Cactus!$F$48,Cactus!$F$51,Cactus!$F$54)</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">(Cactus!$F$4,Cactus!$F$7,Cactus!$F$10,Cactus!$F$13,Cactus!$F$16,Cactus!$F$19,Cactus!$F$20,Cactus!$F$23,Cactus!$F$26,Cactus!$F$29,Cactus!$F$32,Cactus!$F$35,Cactus!$F$40,Cactus!$F$43,Cactus!$F$46,Cactus!$F$49,Cactus!$F$52,Cactus!$F$55)</definedName>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1967" uniqueCount="193">
   <si>
     <t>Well Position</t>
   </si>
@@ -646,6 +648,9 @@
   </si>
   <si>
     <t>SD</t>
+  </si>
+  <si>
+    <t>Real</t>
   </si>
 </sst>
 </file>
@@ -14152,7 +14157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4ADEF0-7664-4391-A09C-F24CBB51FD97}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -14936,7 +14941,3768 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5831132A-6213-4CBC-8484-5B92B74FBD42}">
+  <dimension ref="A1:I217"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E218" sqref="E218"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="5.40625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.04296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6796875" style="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1.4968999999999999</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D3" s="8">
+        <v>4.4233000000000002</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="8">
+        <v>51.712000000000003</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1.2423</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4.2953999999999999</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" s="8">
+        <v>20.6371</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A8">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1.1293</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A9">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2.4594</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" s="8">
+        <v>44.673900000000003</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A11">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1.2533000000000001</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A12">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" s="8">
+        <v>13.443899999999999</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A13">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D13" s="8">
+        <v>32.5351</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A14">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="8" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A15">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2.9918</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A16">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" t="s">
+        <v>190</v>
+      </c>
+      <c r="D16" s="8">
+        <v>17.4602</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A17">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.61080000000000001</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A18">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" t="s">
+        <v>190</v>
+      </c>
+      <c r="D18" s="8" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A19">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C19" t="s">
+        <v>190</v>
+      </c>
+      <c r="D19" s="8" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A20">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20" t="s">
+        <v>190</v>
+      </c>
+      <c r="D20" s="8">
+        <v>11.2843</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A21">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" t="s">
+        <v>190</v>
+      </c>
+      <c r="D21" s="8">
+        <v>2.3896000000000002</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" t="s">
+        <v>190</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.75360000000000005</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A23">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" t="s">
+        <v>190</v>
+      </c>
+      <c r="D23" s="8">
+        <v>8.2329000000000008</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A24">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" t="s">
+        <v>190</v>
+      </c>
+      <c r="D24" s="8">
+        <v>4.6044999999999998</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A25">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" t="s">
+        <v>190</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0.79220000000000002</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A26">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" t="s">
+        <v>190</v>
+      </c>
+      <c r="D26" s="8">
+        <v>11.7745</v>
+      </c>
+      <c r="E26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A27">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>180</v>
+      </c>
+      <c r="C27" t="s">
+        <v>190</v>
+      </c>
+      <c r="D27" s="8">
+        <v>8.2761999999999993</v>
+      </c>
+      <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A28">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>179</v>
+      </c>
+      <c r="C28" t="s">
+        <v>190</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0.32969999999999999</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A29">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>181</v>
+      </c>
+      <c r="C29" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29" s="8">
+        <v>6.7778999999999998</v>
+      </c>
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>180</v>
+      </c>
+      <c r="C30" t="s">
+        <v>190</v>
+      </c>
+      <c r="D30" s="8">
+        <v>3.2662</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" t="s">
+        <v>190</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1.1875</v>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>181</v>
+      </c>
+      <c r="C32" t="s">
+        <v>190</v>
+      </c>
+      <c r="D32" s="8">
+        <v>27.4818</v>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>180</v>
+      </c>
+      <c r="C33" t="s">
+        <v>190</v>
+      </c>
+      <c r="D33" s="8" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>179</v>
+      </c>
+      <c r="C34" t="s">
+        <v>190</v>
+      </c>
+      <c r="D34" s="8">
+        <v>2.5034999999999998</v>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35" t="s">
+        <v>181</v>
+      </c>
+      <c r="C35" t="s">
+        <v>190</v>
+      </c>
+      <c r="D35" s="8">
+        <v>0.62280000000000002</v>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A36">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>180</v>
+      </c>
+      <c r="C36" t="s">
+        <v>190</v>
+      </c>
+      <c r="D36" s="8" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A37">
+        <v>30</v>
+      </c>
+      <c r="B37" t="s">
+        <v>179</v>
+      </c>
+      <c r="C37" t="s">
+        <v>190</v>
+      </c>
+      <c r="D37" s="8">
+        <v>1</v>
+      </c>
+      <c r="E37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="8"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" t="s">
+        <v>190</v>
+      </c>
+      <c r="D38" s="8">
+        <v>1.4032</v>
+      </c>
+      <c r="E38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A39">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" t="s">
+        <v>190</v>
+      </c>
+      <c r="D39" s="8">
+        <v>0.84630000000000005</v>
+      </c>
+      <c r="E39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A40">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>181</v>
+      </c>
+      <c r="C40" t="s">
+        <v>190</v>
+      </c>
+      <c r="D40" s="8">
+        <v>22.253799999999998</v>
+      </c>
+      <c r="E40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A41">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41" t="s">
+        <v>190</v>
+      </c>
+      <c r="D41" s="8">
+        <v>1.9323999999999999</v>
+      </c>
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A42">
+        <v>34</v>
+      </c>
+      <c r="B42" t="s">
+        <v>180</v>
+      </c>
+      <c r="C42" t="s">
+        <v>190</v>
+      </c>
+      <c r="D42" s="8">
+        <v>2.8921000000000001</v>
+      </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A43">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>181</v>
+      </c>
+      <c r="C43" t="s">
+        <v>190</v>
+      </c>
+      <c r="D43" s="8">
+        <v>11.955500000000001</v>
+      </c>
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A44">
+        <v>34</v>
+      </c>
+      <c r="B44" t="s">
+        <v>179</v>
+      </c>
+      <c r="C44" t="s">
+        <v>190</v>
+      </c>
+      <c r="D44" s="8">
+        <v>0.91059999999999997</v>
+      </c>
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A45">
+        <v>34</v>
+      </c>
+      <c r="B45" t="s">
+        <v>180</v>
+      </c>
+      <c r="C45" t="s">
+        <v>190</v>
+      </c>
+      <c r="D45" s="8">
+        <v>2.4357000000000002</v>
+      </c>
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A46">
+        <v>34</v>
+      </c>
+      <c r="B46" t="s">
+        <v>181</v>
+      </c>
+      <c r="C46" t="s">
+        <v>190</v>
+      </c>
+      <c r="D46" s="8">
+        <v>10.7469</v>
+      </c>
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A47">
+        <v>34</v>
+      </c>
+      <c r="B47" t="s">
+        <v>179</v>
+      </c>
+      <c r="C47" t="s">
+        <v>190</v>
+      </c>
+      <c r="D47" s="8">
+        <v>2.6364000000000001</v>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A48">
+        <v>34</v>
+      </c>
+      <c r="B48" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" t="s">
+        <v>190</v>
+      </c>
+      <c r="D48" s="8">
+        <v>2.3853</v>
+      </c>
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A49">
+        <v>34</v>
+      </c>
+      <c r="B49" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" t="s">
+        <v>190</v>
+      </c>
+      <c r="D49" s="8">
+        <v>6.4763999999999999</v>
+      </c>
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A50">
+        <v>34</v>
+      </c>
+      <c r="B50" t="s">
+        <v>179</v>
+      </c>
+      <c r="C50" t="s">
+        <v>190</v>
+      </c>
+      <c r="D50" s="8" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A51">
+        <v>34</v>
+      </c>
+      <c r="B51" t="s">
+        <v>180</v>
+      </c>
+      <c r="C51" t="s">
+        <v>190</v>
+      </c>
+      <c r="D51" s="8">
+        <v>4.8316999999999997</v>
+      </c>
+      <c r="E51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A52">
+        <v>34</v>
+      </c>
+      <c r="B52" t="s">
+        <v>181</v>
+      </c>
+      <c r="C52" t="s">
+        <v>190</v>
+      </c>
+      <c r="D52" s="8" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A53">
+        <v>34</v>
+      </c>
+      <c r="B53" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" t="s">
+        <v>190</v>
+      </c>
+      <c r="D53" s="8">
+        <v>1.0620000000000001</v>
+      </c>
+      <c r="E53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A54">
+        <v>34</v>
+      </c>
+      <c r="B54" t="s">
+        <v>180</v>
+      </c>
+      <c r="C54" t="s">
+        <v>190</v>
+      </c>
+      <c r="D54" s="8" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A55">
+        <v>34</v>
+      </c>
+      <c r="B55" t="s">
+        <v>181</v>
+      </c>
+      <c r="C55" t="s">
+        <v>190</v>
+      </c>
+      <c r="D55" s="8">
+        <v>2.0011000000000001</v>
+      </c>
+      <c r="E55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A56">
+        <v>24</v>
+      </c>
+      <c r="B56" t="s">
+        <v>181</v>
+      </c>
+      <c r="C56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D56" s="8">
+        <v>7.8946562297804608</v>
+      </c>
+      <c r="E56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A57">
+        <v>24</v>
+      </c>
+      <c r="B57" t="s">
+        <v>181</v>
+      </c>
+      <c r="C57" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57" s="8">
+        <v>14.481835483829794</v>
+      </c>
+      <c r="E57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A58">
+        <v>24</v>
+      </c>
+      <c r="B58" t="s">
+        <v>181</v>
+      </c>
+      <c r="C58" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="8">
+        <v>24.361494941271186</v>
+      </c>
+      <c r="E58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A59">
+        <v>24</v>
+      </c>
+      <c r="B59" t="s">
+        <v>181</v>
+      </c>
+      <c r="C59" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" s="8">
+        <v>15.152738980383106</v>
+      </c>
+      <c r="E59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A60">
+        <v>24</v>
+      </c>
+      <c r="B60" t="s">
+        <v>181</v>
+      </c>
+      <c r="C60" t="s">
+        <v>56</v>
+      </c>
+      <c r="D60" s="8">
+        <v>14.064169384750608</v>
+      </c>
+      <c r="E60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A61">
+        <v>24</v>
+      </c>
+      <c r="B61" t="s">
+        <v>181</v>
+      </c>
+      <c r="C61" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="8">
+        <v>16.2611850143198</v>
+      </c>
+      <c r="E61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A62">
+        <v>30</v>
+      </c>
+      <c r="B62" t="s">
+        <v>181</v>
+      </c>
+      <c r="C62" t="s">
+        <v>56</v>
+      </c>
+      <c r="D62" s="8">
+        <v>2.104708330835265</v>
+      </c>
+      <c r="E62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A63">
+        <v>30</v>
+      </c>
+      <c r="B63" t="s">
+        <v>181</v>
+      </c>
+      <c r="C63" t="s">
+        <v>56</v>
+      </c>
+      <c r="D63" s="8">
+        <v>3.3498875104733572</v>
+      </c>
+      <c r="E63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A64">
+        <v>30</v>
+      </c>
+      <c r="B64" t="s">
+        <v>181</v>
+      </c>
+      <c r="C64" t="s">
+        <v>56</v>
+      </c>
+      <c r="D64" s="8">
+        <v>8.3346560134937437</v>
+      </c>
+      <c r="E64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A65">
+        <v>30</v>
+      </c>
+      <c r="B65" t="s">
+        <v>181</v>
+      </c>
+      <c r="C65" t="s">
+        <v>56</v>
+      </c>
+      <c r="D65" s="8">
+        <v>6.3330896749643468</v>
+      </c>
+      <c r="E65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A66">
+        <v>30</v>
+      </c>
+      <c r="B66" t="s">
+        <v>181</v>
+      </c>
+      <c r="C66" t="s">
+        <v>56</v>
+      </c>
+      <c r="D66" s="8">
+        <v>0.82715430662305678</v>
+      </c>
+      <c r="E66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A67">
+        <v>30</v>
+      </c>
+      <c r="B67" t="s">
+        <v>181</v>
+      </c>
+      <c r="C67" t="s">
+        <v>56</v>
+      </c>
+      <c r="D67" s="8">
+        <v>12.334761785472088</v>
+      </c>
+      <c r="E67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A68">
+        <v>34</v>
+      </c>
+      <c r="B68" t="s">
+        <v>181</v>
+      </c>
+      <c r="C68" t="s">
+        <v>56</v>
+      </c>
+      <c r="D68" s="8">
+        <v>3.6094678070349264</v>
+      </c>
+      <c r="E68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A69">
+        <v>34</v>
+      </c>
+      <c r="B69" t="s">
+        <v>181</v>
+      </c>
+      <c r="C69" t="s">
+        <v>56</v>
+      </c>
+      <c r="D69" s="8">
+        <v>2.7918753888697498</v>
+      </c>
+      <c r="E69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A70">
+        <v>34</v>
+      </c>
+      <c r="B70" t="s">
+        <v>181</v>
+      </c>
+      <c r="C70" t="s">
+        <v>56</v>
+      </c>
+      <c r="D70" s="8">
+        <v>5.4068671167230633</v>
+      </c>
+      <c r="E70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A71">
+        <v>34</v>
+      </c>
+      <c r="B71" t="s">
+        <v>181</v>
+      </c>
+      <c r="C71" t="s">
+        <v>56</v>
+      </c>
+      <c r="D71" s="8">
+        <v>5.3465188279580493</v>
+      </c>
+      <c r="E71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A72">
+        <v>34</v>
+      </c>
+      <c r="B72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C72" t="s">
+        <v>56</v>
+      </c>
+      <c r="D72" s="8">
+        <v>3.6929674993635762</v>
+      </c>
+      <c r="E72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A73">
+        <v>34</v>
+      </c>
+      <c r="B73" t="s">
+        <v>181</v>
+      </c>
+      <c r="C73" t="s">
+        <v>56</v>
+      </c>
+      <c r="D73" s="8">
+        <v>9.3261924731057331</v>
+      </c>
+      <c r="E73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A74">
+        <v>24</v>
+      </c>
+      <c r="B74" t="s">
+        <v>180</v>
+      </c>
+      <c r="C74" t="s">
+        <v>56</v>
+      </c>
+      <c r="D74" s="8">
+        <v>0.96213143518723743</v>
+      </c>
+      <c r="E74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A75">
+        <v>24</v>
+      </c>
+      <c r="B75" t="s">
+        <v>180</v>
+      </c>
+      <c r="C75" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" s="8">
+        <v>1.4737256300434598</v>
+      </c>
+      <c r="E75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A76">
+        <v>24</v>
+      </c>
+      <c r="B76" t="s">
+        <v>180</v>
+      </c>
+      <c r="C76" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" s="8">
+        <v>3.6382955661108567</v>
+      </c>
+      <c r="E76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A77">
+        <v>24</v>
+      </c>
+      <c r="B77" t="s">
+        <v>180</v>
+      </c>
+      <c r="C77" t="s">
+        <v>56</v>
+      </c>
+      <c r="D77" s="8">
+        <v>1.7715186435860284</v>
+      </c>
+      <c r="E77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A78">
+        <v>24</v>
+      </c>
+      <c r="B78" t="s">
+        <v>180</v>
+      </c>
+      <c r="C78" t="s">
+        <v>56</v>
+      </c>
+      <c r="D78" s="8">
+        <v>4.2464482339861025</v>
+      </c>
+      <c r="E78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A79">
+        <v>24</v>
+      </c>
+      <c r="B79" t="s">
+        <v>180</v>
+      </c>
+      <c r="C79" t="s">
+        <v>56</v>
+      </c>
+      <c r="D79" s="8">
+        <v>2.0083172225988659</v>
+      </c>
+      <c r="E79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A80">
+        <v>30</v>
+      </c>
+      <c r="B80" t="s">
+        <v>180</v>
+      </c>
+      <c r="C80" t="s">
+        <v>56</v>
+      </c>
+      <c r="D80" s="8">
+        <v>1.0067513807074795</v>
+      </c>
+      <c r="E80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A81">
+        <v>30</v>
+      </c>
+      <c r="B81" t="s">
+        <v>180</v>
+      </c>
+      <c r="C81" t="s">
+        <v>56</v>
+      </c>
+      <c r="D81" s="8">
+        <v>1.3860580087485403</v>
+      </c>
+      <c r="E81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A82">
+        <v>30</v>
+      </c>
+      <c r="B82" t="s">
+        <v>180</v>
+      </c>
+      <c r="C82" t="s">
+        <v>56</v>
+      </c>
+      <c r="D82" s="8">
+        <v>2.6895728770310723</v>
+      </c>
+      <c r="E82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A83">
+        <v>30</v>
+      </c>
+      <c r="B83" t="s">
+        <v>180</v>
+      </c>
+      <c r="C83" t="s">
+        <v>56</v>
+      </c>
+      <c r="D83" s="8">
+        <v>2.3511568400627958</v>
+      </c>
+      <c r="E83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A84">
+        <v>30</v>
+      </c>
+      <c r="B84" t="s">
+        <v>180</v>
+      </c>
+      <c r="C84" t="s">
+        <v>56</v>
+      </c>
+      <c r="D84" s="8">
+        <v>0.50608861879188216</v>
+      </c>
+      <c r="E84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A85">
+        <v>30</v>
+      </c>
+      <c r="B85" t="s">
+        <v>180</v>
+      </c>
+      <c r="C85" t="s">
+        <v>56</v>
+      </c>
+      <c r="D85" s="8">
+        <v>1.2252027301372606</v>
+      </c>
+      <c r="E85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A86">
+        <v>34</v>
+      </c>
+      <c r="B86" t="s">
+        <v>180</v>
+      </c>
+      <c r="C86" t="s">
+        <v>56</v>
+      </c>
+      <c r="D86" s="8">
+        <v>0.85082728788912254</v>
+      </c>
+      <c r="E86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A87">
+        <v>34</v>
+      </c>
+      <c r="B87" t="s">
+        <v>180</v>
+      </c>
+      <c r="C87" t="s">
+        <v>56</v>
+      </c>
+      <c r="D87" s="8">
+        <v>1.346984228248381</v>
+      </c>
+      <c r="E87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A88">
+        <v>34</v>
+      </c>
+      <c r="B88" t="s">
+        <v>180</v>
+      </c>
+      <c r="C88" t="s">
+        <v>56</v>
+      </c>
+      <c r="D88" s="8">
+        <v>1.1416457045871948</v>
+      </c>
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A89">
+        <v>34</v>
+      </c>
+      <c r="B89" t="s">
+        <v>180</v>
+      </c>
+      <c r="C89" t="s">
+        <v>56</v>
+      </c>
+      <c r="D89" s="8">
+        <v>2.2179897537201985</v>
+      </c>
+      <c r="E89" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A90">
+        <v>34</v>
+      </c>
+      <c r="B90" t="s">
+        <v>180</v>
+      </c>
+      <c r="C90" t="s">
+        <v>56</v>
+      </c>
+      <c r="D90" s="8">
+        <v>0.90256600508903417</v>
+      </c>
+      <c r="E90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A91">
+        <v>34</v>
+      </c>
+      <c r="B91" t="s">
+        <v>180</v>
+      </c>
+      <c r="C91" t="s">
+        <v>56</v>
+      </c>
+      <c r="D91" s="8">
+        <v>1.2134040618405697</v>
+      </c>
+      <c r="E91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A92">
+        <v>24</v>
+      </c>
+      <c r="B92" t="s">
+        <v>179</v>
+      </c>
+      <c r="C92" t="s">
+        <v>56</v>
+      </c>
+      <c r="D92" s="8">
+        <v>0.43855295526547822</v>
+      </c>
+      <c r="E92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A93">
+        <v>24</v>
+      </c>
+      <c r="B93" t="s">
+        <v>179</v>
+      </c>
+      <c r="C93" t="s">
+        <v>56</v>
+      </c>
+      <c r="D93" s="8">
+        <v>1.1177255689618641</v>
+      </c>
+      <c r="E93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A94">
+        <v>24</v>
+      </c>
+      <c r="B94" t="s">
+        <v>179</v>
+      </c>
+      <c r="C94" t="s">
+        <v>56</v>
+      </c>
+      <c r="D94" s="8">
+        <v>2.0667359487642689</v>
+      </c>
+      <c r="E94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A95">
+        <v>24</v>
+      </c>
+      <c r="B95" t="s">
+        <v>179</v>
+      </c>
+      <c r="C95" t="s">
+        <v>56</v>
+      </c>
+      <c r="D95" s="8">
+        <v>2.8961306029909482</v>
+      </c>
+      <c r="E95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A96">
+        <v>24</v>
+      </c>
+      <c r="B96" t="s">
+        <v>179</v>
+      </c>
+      <c r="C96" t="s">
+        <v>56</v>
+      </c>
+      <c r="D96" s="8">
+        <v>1.1522121853461109</v>
+      </c>
+      <c r="E96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A97">
+        <v>24</v>
+      </c>
+      <c r="B97" t="s">
+        <v>179</v>
+      </c>
+      <c r="C97" t="s">
+        <v>56</v>
+      </c>
+      <c r="D97" s="8">
+        <v>3.8830035590545724</v>
+      </c>
+      <c r="E97" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A98">
+        <v>30</v>
+      </c>
+      <c r="B98" t="s">
+        <v>179</v>
+      </c>
+      <c r="C98" t="s">
+        <v>56</v>
+      </c>
+      <c r="D98" s="8">
+        <v>1</v>
+      </c>
+      <c r="E98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A99">
+        <v>30</v>
+      </c>
+      <c r="B99" t="s">
+        <v>179</v>
+      </c>
+      <c r="C99" t="s">
+        <v>56</v>
+      </c>
+      <c r="D99" s="8">
+        <v>1</v>
+      </c>
+      <c r="E99" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A100">
+        <v>30</v>
+      </c>
+      <c r="B100" t="s">
+        <v>179</v>
+      </c>
+      <c r="C100" t="s">
+        <v>56</v>
+      </c>
+      <c r="D100" s="8">
+        <v>1</v>
+      </c>
+      <c r="E100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A101">
+        <v>30</v>
+      </c>
+      <c r="B101" t="s">
+        <v>179</v>
+      </c>
+      <c r="C101" t="s">
+        <v>56</v>
+      </c>
+      <c r="D101" s="8">
+        <v>1</v>
+      </c>
+      <c r="E101" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A102">
+        <v>30</v>
+      </c>
+      <c r="B102" t="s">
+        <v>179</v>
+      </c>
+      <c r="C102" t="s">
+        <v>56</v>
+      </c>
+      <c r="D102" s="8">
+        <v>1</v>
+      </c>
+      <c r="E102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A103">
+        <v>30</v>
+      </c>
+      <c r="B103" t="s">
+        <v>179</v>
+      </c>
+      <c r="C103" t="s">
+        <v>56</v>
+      </c>
+      <c r="D103" s="8">
+        <v>1</v>
+      </c>
+      <c r="E103" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A104">
+        <v>34</v>
+      </c>
+      <c r="B104" t="s">
+        <v>179</v>
+      </c>
+      <c r="C104" t="s">
+        <v>56</v>
+      </c>
+      <c r="D104" s="8">
+        <v>1.1135763535298939</v>
+      </c>
+      <c r="E104" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A105">
+        <v>34</v>
+      </c>
+      <c r="B105" t="s">
+        <v>179</v>
+      </c>
+      <c r="C105" t="s">
+        <v>56</v>
+      </c>
+      <c r="D105" s="8">
+        <v>1.2512624673819928</v>
+      </c>
+      <c r="E105" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A106">
+        <v>34</v>
+      </c>
+      <c r="B106" t="s">
+        <v>179</v>
+      </c>
+      <c r="C106" t="s">
+        <v>56</v>
+      </c>
+      <c r="D106" s="8">
+        <v>1.2449164792330876</v>
+      </c>
+      <c r="E106" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A107">
+        <v>34</v>
+      </c>
+      <c r="B107" t="s">
+        <v>179</v>
+      </c>
+      <c r="C107" t="s">
+        <v>56</v>
+      </c>
+      <c r="D107" s="8">
+        <v>0.91655104059714321</v>
+      </c>
+      <c r="E107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A108">
+        <v>34</v>
+      </c>
+      <c r="B108" t="s">
+        <v>179</v>
+      </c>
+      <c r="C108" t="s">
+        <v>56</v>
+      </c>
+      <c r="D108" s="8">
+        <v>1.0165373350044271</v>
+      </c>
+      <c r="E108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A109">
+        <v>34</v>
+      </c>
+      <c r="B109" t="s">
+        <v>179</v>
+      </c>
+      <c r="C109" t="s">
+        <v>56</v>
+      </c>
+      <c r="D109" s="8">
+        <v>0.98444900580502814</v>
+      </c>
+      <c r="E109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A110">
+        <v>24</v>
+      </c>
+      <c r="B110" t="s">
+        <v>179</v>
+      </c>
+      <c r="C110" t="s">
+        <v>162</v>
+      </c>
+      <c r="D110" s="8">
+        <v>2.1242971520355334</v>
+      </c>
+      <c r="E110" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A111">
+        <v>24</v>
+      </c>
+      <c r="B111" t="s">
+        <v>180</v>
+      </c>
+      <c r="C111" t="s">
+        <v>162</v>
+      </c>
+      <c r="D111" s="8">
+        <v>4.291706844760796</v>
+      </c>
+      <c r="E111" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A112">
+        <v>24</v>
+      </c>
+      <c r="B112" t="s">
+        <v>181</v>
+      </c>
+      <c r="C112" t="s">
+        <v>162</v>
+      </c>
+      <c r="D112" s="8">
+        <v>4.0973316061281428</v>
+      </c>
+      <c r="E112" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A113">
+        <v>24</v>
+      </c>
+      <c r="B113" t="s">
+        <v>179</v>
+      </c>
+      <c r="C113" t="s">
+        <v>162</v>
+      </c>
+      <c r="D113" s="8">
+        <v>1.4003082825932121</v>
+      </c>
+      <c r="E113" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A114">
+        <v>24</v>
+      </c>
+      <c r="B114" t="s">
+        <v>180</v>
+      </c>
+      <c r="C114" t="s">
+        <v>162</v>
+      </c>
+      <c r="D114" s="8">
+        <v>4.2822781418585629</v>
+      </c>
+      <c r="E114" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A115">
+        <v>24</v>
+      </c>
+      <c r="B115" t="s">
+        <v>181</v>
+      </c>
+      <c r="C115" t="s">
+        <v>162</v>
+      </c>
+      <c r="D115" s="8">
+        <v>24.879857304108231</v>
+      </c>
+      <c r="E115" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A116">
+        <v>24</v>
+      </c>
+      <c r="B116" t="s">
+        <v>179</v>
+      </c>
+      <c r="C116" t="s">
+        <v>162</v>
+      </c>
+      <c r="D116" s="8">
+        <v>2.1361512628337644</v>
+      </c>
+      <c r="E116" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A117">
+        <v>24</v>
+      </c>
+      <c r="B117" t="s">
+        <v>180</v>
+      </c>
+      <c r="C117" t="s">
+        <v>162</v>
+      </c>
+      <c r="D117" s="8">
+        <v>4.4234725395964745</v>
+      </c>
+      <c r="E117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A118">
+        <v>24</v>
+      </c>
+      <c r="B118" t="s">
+        <v>181</v>
+      </c>
+      <c r="C118" t="s">
+        <v>162</v>
+      </c>
+      <c r="D118" s="8">
+        <v>24.233747546798313</v>
+      </c>
+      <c r="E118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A119">
+        <v>24</v>
+      </c>
+      <c r="B119" t="s">
+        <v>179</v>
+      </c>
+      <c r="C119" t="s">
+        <v>162</v>
+      </c>
+      <c r="D119" s="8">
+        <v>2.4320009352248682</v>
+      </c>
+      <c r="E119" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A120">
+        <v>24</v>
+      </c>
+      <c r="B120" t="s">
+        <v>180</v>
+      </c>
+      <c r="C120" t="s">
+        <v>162</v>
+      </c>
+      <c r="D120" s="8">
+        <v>3.2087767766407076</v>
+      </c>
+      <c r="E120" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A121">
+        <v>24</v>
+      </c>
+      <c r="B121" t="s">
+        <v>181</v>
+      </c>
+      <c r="C121" t="s">
+        <v>162</v>
+      </c>
+      <c r="D121" s="8">
+        <v>11.923025326389997</v>
+      </c>
+      <c r="E121" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A122">
+        <v>24</v>
+      </c>
+      <c r="B122" t="s">
+        <v>179</v>
+      </c>
+      <c r="C122" t="s">
+        <v>162</v>
+      </c>
+      <c r="D122" s="8">
+        <v>4.0303255151733959</v>
+      </c>
+      <c r="E122" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A123">
+        <v>24</v>
+      </c>
+      <c r="B123" t="s">
+        <v>180</v>
+      </c>
+      <c r="C123" t="s">
+        <v>162</v>
+      </c>
+      <c r="D123" s="8">
+        <v>5.4793397531315007</v>
+      </c>
+      <c r="E123" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A124">
+        <v>24</v>
+      </c>
+      <c r="B124" t="s">
+        <v>181</v>
+      </c>
+      <c r="C124" t="s">
+        <v>162</v>
+      </c>
+      <c r="D124" s="8">
+        <v>3.8660381950190703</v>
+      </c>
+      <c r="E124" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A125">
+        <v>24</v>
+      </c>
+      <c r="B125" t="s">
+        <v>179</v>
+      </c>
+      <c r="C125" t="s">
+        <v>162</v>
+      </c>
+      <c r="D125" s="8">
+        <v>0.78798330374844805</v>
+      </c>
+      <c r="E125" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A126">
+        <v>24</v>
+      </c>
+      <c r="B126" t="s">
+        <v>180</v>
+      </c>
+      <c r="C126" t="s">
+        <v>162</v>
+      </c>
+      <c r="D126" s="8">
+        <v>4.1156288923036524</v>
+      </c>
+      <c r="E126" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A127">
+        <v>24</v>
+      </c>
+      <c r="B127" t="s">
+        <v>181</v>
+      </c>
+      <c r="C127" t="s">
+        <v>162</v>
+      </c>
+      <c r="D127" s="8">
+        <v>17.584575159373117</v>
+      </c>
+      <c r="E127" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A128">
+        <v>30</v>
+      </c>
+      <c r="B128" t="s">
+        <v>181</v>
+      </c>
+      <c r="C128" t="s">
+        <v>162</v>
+      </c>
+      <c r="D128" s="8">
+        <v>0.62926575287712383</v>
+      </c>
+      <c r="E128" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A129">
+        <v>30</v>
+      </c>
+      <c r="B129" t="s">
+        <v>180</v>
+      </c>
+      <c r="C129" t="s">
+        <v>162</v>
+      </c>
+      <c r="D129" s="8">
+        <v>1.4813329696016226</v>
+      </c>
+      <c r="E129" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A130">
+        <v>30</v>
+      </c>
+      <c r="B130" t="s">
+        <v>179</v>
+      </c>
+      <c r="C130" t="s">
+        <v>162</v>
+      </c>
+      <c r="D130" s="8">
+        <v>1</v>
+      </c>
+      <c r="E130" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A131">
+        <v>30</v>
+      </c>
+      <c r="B131" t="s">
+        <v>181</v>
+      </c>
+      <c r="C131" t="s">
+        <v>162</v>
+      </c>
+      <c r="D131" s="8">
+        <v>8.4712330715386397</v>
+      </c>
+      <c r="E131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A132">
+        <v>30</v>
+      </c>
+      <c r="B132" t="s">
+        <v>180</v>
+      </c>
+      <c r="C132" t="s">
+        <v>162</v>
+      </c>
+      <c r="D132" s="8">
+        <v>2.193379100598857</v>
+      </c>
+      <c r="E132" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A133">
+        <v>30</v>
+      </c>
+      <c r="B133" t="s">
+        <v>179</v>
+      </c>
+      <c r="C133" t="s">
+        <v>162</v>
+      </c>
+      <c r="D133" s="8">
+        <v>1</v>
+      </c>
+      <c r="E133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A134">
+        <v>30</v>
+      </c>
+      <c r="B134" t="s">
+        <v>181</v>
+      </c>
+      <c r="C134" t="s">
+        <v>162</v>
+      </c>
+      <c r="D134" s="8">
+        <v>7.2401684522156904</v>
+      </c>
+      <c r="E134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A135">
+        <v>30</v>
+      </c>
+      <c r="B135" t="s">
+        <v>180</v>
+      </c>
+      <c r="C135" t="s">
+        <v>162</v>
+      </c>
+      <c r="D135" s="8">
+        <v>2.8798616356860864</v>
+      </c>
+      <c r="E135" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A136">
+        <v>30</v>
+      </c>
+      <c r="B136" t="s">
+        <v>179</v>
+      </c>
+      <c r="C136" t="s">
+        <v>162</v>
+      </c>
+      <c r="D136" s="8">
+        <v>1</v>
+      </c>
+      <c r="E136" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A137">
+        <v>30</v>
+      </c>
+      <c r="B137" t="s">
+        <v>181</v>
+      </c>
+      <c r="C137" t="s">
+        <v>162</v>
+      </c>
+      <c r="D137" s="8">
+        <v>4.9186883858404551</v>
+      </c>
+      <c r="E137" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A138">
+        <v>30</v>
+      </c>
+      <c r="B138" t="s">
+        <v>180</v>
+      </c>
+      <c r="C138" t="s">
+        <v>162</v>
+      </c>
+      <c r="D138" s="8">
+        <v>2.4557101522683311</v>
+      </c>
+      <c r="E138" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A139">
+        <v>30</v>
+      </c>
+      <c r="B139" t="s">
+        <v>179</v>
+      </c>
+      <c r="C139" t="s">
+        <v>162</v>
+      </c>
+      <c r="D139" s="8">
+        <v>1</v>
+      </c>
+      <c r="E139" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A140">
+        <v>30</v>
+      </c>
+      <c r="B140" t="s">
+        <v>181</v>
+      </c>
+      <c r="C140" t="s">
+        <v>162</v>
+      </c>
+      <c r="D140" s="8">
+        <v>6.6619319408771291</v>
+      </c>
+      <c r="E140" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A141">
+        <v>30</v>
+      </c>
+      <c r="B141" t="s">
+        <v>180</v>
+      </c>
+      <c r="C141" t="s">
+        <v>162</v>
+      </c>
+      <c r="D141" s="8">
+        <v>1.1542815525474373</v>
+      </c>
+      <c r="E141" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A142">
+        <v>30</v>
+      </c>
+      <c r="B142" t="s">
+        <v>179</v>
+      </c>
+      <c r="C142" t="s">
+        <v>162</v>
+      </c>
+      <c r="D142" s="8">
+        <v>1</v>
+      </c>
+      <c r="E142" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A143">
+        <v>30</v>
+      </c>
+      <c r="B143" t="s">
+        <v>181</v>
+      </c>
+      <c r="C143" t="s">
+        <v>162</v>
+      </c>
+      <c r="D143" s="8">
+        <v>1.549177517412722</v>
+      </c>
+      <c r="E143" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A144">
+        <v>30</v>
+      </c>
+      <c r="B144" t="s">
+        <v>180</v>
+      </c>
+      <c r="C144" t="s">
+        <v>162</v>
+      </c>
+      <c r="D144" s="8">
+        <v>1.1568740304497094</v>
+      </c>
+      <c r="E144" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A145">
+        <v>30</v>
+      </c>
+      <c r="B145" t="s">
+        <v>179</v>
+      </c>
+      <c r="C145" t="s">
+        <v>162</v>
+      </c>
+      <c r="D145" s="8">
+        <v>1</v>
+      </c>
+      <c r="E145" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A146">
+        <v>34</v>
+      </c>
+      <c r="B146" t="s">
+        <v>179</v>
+      </c>
+      <c r="C146" t="s">
+        <v>162</v>
+      </c>
+      <c r="D146" s="8">
+        <v>0.99202811345468989</v>
+      </c>
+      <c r="E146" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A147">
+        <v>34</v>
+      </c>
+      <c r="B147" t="s">
+        <v>180</v>
+      </c>
+      <c r="C147" t="s">
+        <v>162</v>
+      </c>
+      <c r="D147" s="8">
+        <v>2.9354500638805625</v>
+      </c>
+      <c r="E147" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A148">
+        <v>34</v>
+      </c>
+      <c r="B148" t="s">
+        <v>181</v>
+      </c>
+      <c r="C148" t="s">
+        <v>162</v>
+      </c>
+      <c r="D148" s="8">
+        <v>24.403576764692222</v>
+      </c>
+      <c r="E148" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A149">
+        <v>34</v>
+      </c>
+      <c r="B149" t="s">
+        <v>179</v>
+      </c>
+      <c r="C149" t="s">
+        <v>162</v>
+      </c>
+      <c r="D149" s="8">
+        <v>1.1534283003134</v>
+      </c>
+      <c r="E149" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A150">
+        <v>34</v>
+      </c>
+      <c r="B150" t="s">
+        <v>180</v>
+      </c>
+      <c r="C150" t="s">
+        <v>162</v>
+      </c>
+      <c r="D150" s="8">
+        <v>1.6447935076908315</v>
+      </c>
+      <c r="E150" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A151">
+        <v>34</v>
+      </c>
+      <c r="B151" t="s">
+        <v>181</v>
+      </c>
+      <c r="C151" t="s">
+        <v>162</v>
+      </c>
+      <c r="D151" s="8">
+        <v>12.04132253526303</v>
+      </c>
+      <c r="E151" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A152">
+        <v>34</v>
+      </c>
+      <c r="B152" t="s">
+        <v>179</v>
+      </c>
+      <c r="C152" t="s">
+        <v>162</v>
+      </c>
+      <c r="D152" s="8">
+        <v>1.4431478418462336</v>
+      </c>
+      <c r="E152" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A153">
+        <v>34</v>
+      </c>
+      <c r="B153" t="s">
+        <v>180</v>
+      </c>
+      <c r="C153" t="s">
+        <v>162</v>
+      </c>
+      <c r="D153" s="8">
+        <v>1.9697043994046894</v>
+      </c>
+      <c r="E153" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A154">
+        <v>34</v>
+      </c>
+      <c r="B154" t="s">
+        <v>181</v>
+      </c>
+      <c r="C154" t="s">
+        <v>162</v>
+      </c>
+      <c r="D154" s="8">
+        <v>8.0077394567386389</v>
+      </c>
+      <c r="E154" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A155">
+        <v>34</v>
+      </c>
+      <c r="B155" t="s">
+        <v>179</v>
+      </c>
+      <c r="C155" t="s">
+        <v>162</v>
+      </c>
+      <c r="D155" s="8">
+        <v>0.73189952870282604</v>
+      </c>
+      <c r="E155" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A156">
+        <v>34</v>
+      </c>
+      <c r="B156" t="s">
+        <v>180</v>
+      </c>
+      <c r="C156" t="s">
+        <v>162</v>
+      </c>
+      <c r="D156" s="8">
+        <v>2.2680177969894908</v>
+      </c>
+      <c r="E156" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A157">
+        <v>34</v>
+      </c>
+      <c r="B157" t="s">
+        <v>181</v>
+      </c>
+      <c r="C157" t="s">
+        <v>162</v>
+      </c>
+      <c r="D157" s="8">
+        <v>2.6709889194904322</v>
+      </c>
+      <c r="E157" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A158">
+        <v>34</v>
+      </c>
+      <c r="B158" t="s">
+        <v>179</v>
+      </c>
+      <c r="C158" t="s">
+        <v>162</v>
+      </c>
+      <c r="D158" s="8">
+        <v>0.65358061447701277</v>
+      </c>
+      <c r="E158" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A159">
+        <v>34</v>
+      </c>
+      <c r="B159" t="s">
+        <v>180</v>
+      </c>
+      <c r="C159" t="s">
+        <v>162</v>
+      </c>
+      <c r="D159" s="8">
+        <v>1.2592706200551125</v>
+      </c>
+      <c r="E159" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A160">
+        <v>34</v>
+      </c>
+      <c r="B160" t="s">
+        <v>181</v>
+      </c>
+      <c r="C160" t="s">
+        <v>162</v>
+      </c>
+      <c r="D160" s="8">
+        <v>2.6209052397289865</v>
+      </c>
+      <c r="E160" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A161">
+        <v>34</v>
+      </c>
+      <c r="B161" t="s">
+        <v>179</v>
+      </c>
+      <c r="C161" t="s">
+        <v>162</v>
+      </c>
+      <c r="D161" s="8">
+        <v>0.59701234632890421</v>
+      </c>
+      <c r="E161" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A162">
+        <v>34</v>
+      </c>
+      <c r="B162" t="s">
+        <v>180</v>
+      </c>
+      <c r="C162" t="s">
+        <v>162</v>
+      </c>
+      <c r="D162" s="8">
+        <v>0.34434875232192103</v>
+      </c>
+      <c r="E162" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A163">
+        <v>34</v>
+      </c>
+      <c r="B163" t="s">
+        <v>181</v>
+      </c>
+      <c r="C163" t="s">
+        <v>162</v>
+      </c>
+      <c r="D163" s="8">
+        <v>1.9804227103587813</v>
+      </c>
+      <c r="E163" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A164">
+        <v>20</v>
+      </c>
+      <c r="B164" t="s">
+        <v>181</v>
+      </c>
+      <c r="C164" t="s">
+        <v>190</v>
+      </c>
+      <c r="D164" s="8">
+        <v>11.2843</v>
+      </c>
+      <c r="E164" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A165">
+        <v>20</v>
+      </c>
+      <c r="B165" t="s">
+        <v>180</v>
+      </c>
+      <c r="C165" t="s">
+        <v>190</v>
+      </c>
+      <c r="D165" s="8">
+        <v>2.3896000000000002</v>
+      </c>
+      <c r="E165" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A166">
+        <v>20</v>
+      </c>
+      <c r="B166" t="s">
+        <v>179</v>
+      </c>
+      <c r="C166" t="s">
+        <v>190</v>
+      </c>
+      <c r="D166" s="8">
+        <v>0.75360000000000005</v>
+      </c>
+      <c r="E166" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A167">
+        <v>20</v>
+      </c>
+      <c r="B167" t="s">
+        <v>181</v>
+      </c>
+      <c r="C167" t="s">
+        <v>190</v>
+      </c>
+      <c r="D167" s="8">
+        <v>8.2329000000000008</v>
+      </c>
+      <c r="E167" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A168">
+        <v>20</v>
+      </c>
+      <c r="B168" t="s">
+        <v>180</v>
+      </c>
+      <c r="C168" t="s">
+        <v>190</v>
+      </c>
+      <c r="D168" s="8">
+        <v>4.6044999999999998</v>
+      </c>
+      <c r="E168" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A169">
+        <v>20</v>
+      </c>
+      <c r="B169" t="s">
+        <v>179</v>
+      </c>
+      <c r="C169" t="s">
+        <v>190</v>
+      </c>
+      <c r="D169" s="8">
+        <v>0.79220000000000002</v>
+      </c>
+      <c r="E169" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A170">
+        <v>20</v>
+      </c>
+      <c r="B170" t="s">
+        <v>181</v>
+      </c>
+      <c r="C170" t="s">
+        <v>190</v>
+      </c>
+      <c r="D170" s="8">
+        <v>11.7745</v>
+      </c>
+      <c r="E170" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A171">
+        <v>20</v>
+      </c>
+      <c r="B171" t="s">
+        <v>180</v>
+      </c>
+      <c r="C171" t="s">
+        <v>190</v>
+      </c>
+      <c r="D171" s="8">
+        <v>8.2761999999999993</v>
+      </c>
+      <c r="E171" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A172">
+        <v>20</v>
+      </c>
+      <c r="B172" t="s">
+        <v>179</v>
+      </c>
+      <c r="C172" t="s">
+        <v>190</v>
+      </c>
+      <c r="D172" s="8">
+        <v>0.32969999999999999</v>
+      </c>
+      <c r="E172" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A173">
+        <v>20</v>
+      </c>
+      <c r="B173" t="s">
+        <v>181</v>
+      </c>
+      <c r="C173" t="s">
+        <v>190</v>
+      </c>
+      <c r="D173" s="8">
+        <v>6.7778999999999998</v>
+      </c>
+      <c r="E173" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A174">
+        <v>20</v>
+      </c>
+      <c r="B174" t="s">
+        <v>180</v>
+      </c>
+      <c r="C174" t="s">
+        <v>190</v>
+      </c>
+      <c r="D174" s="8">
+        <v>3.2662</v>
+      </c>
+      <c r="E174" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A175">
+        <v>20</v>
+      </c>
+      <c r="B175" t="s">
+        <v>179</v>
+      </c>
+      <c r="C175" t="s">
+        <v>190</v>
+      </c>
+      <c r="D175" s="8">
+        <v>1.1875</v>
+      </c>
+      <c r="E175" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A176">
+        <v>20</v>
+      </c>
+      <c r="B176" t="s">
+        <v>181</v>
+      </c>
+      <c r="C176" t="s">
+        <v>190</v>
+      </c>
+      <c r="D176" s="8">
+        <v>27.4818</v>
+      </c>
+      <c r="E176" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A177">
+        <v>20</v>
+      </c>
+      <c r="B177" t="s">
+        <v>180</v>
+      </c>
+      <c r="C177" t="s">
+        <v>190</v>
+      </c>
+      <c r="D177" s="8" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E177" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A178">
+        <v>20</v>
+      </c>
+      <c r="B178" t="s">
+        <v>179</v>
+      </c>
+      <c r="C178" t="s">
+        <v>190</v>
+      </c>
+      <c r="D178" s="8">
+        <v>2.5034999999999998</v>
+      </c>
+      <c r="E178" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A179">
+        <v>20</v>
+      </c>
+      <c r="B179" t="s">
+        <v>181</v>
+      </c>
+      <c r="C179" t="s">
+        <v>190</v>
+      </c>
+      <c r="D179" s="8">
+        <v>0.62280000000000002</v>
+      </c>
+      <c r="E179" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A180">
+        <v>20</v>
+      </c>
+      <c r="B180" t="s">
+        <v>180</v>
+      </c>
+      <c r="C180" t="s">
+        <v>190</v>
+      </c>
+      <c r="D180" s="8" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="E180" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A181">
+        <v>20</v>
+      </c>
+      <c r="B181" t="s">
+        <v>179</v>
+      </c>
+      <c r="C181" t="s">
+        <v>190</v>
+      </c>
+      <c r="D181" s="8">
+        <v>1</v>
+      </c>
+      <c r="E181" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A182">
+        <v>20</v>
+      </c>
+      <c r="B182" t="s">
+        <v>181</v>
+      </c>
+      <c r="C182" t="s">
+        <v>56</v>
+      </c>
+      <c r="D182" s="8">
+        <v>2.104708330835265</v>
+      </c>
+      <c r="E182" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A183">
+        <v>20</v>
+      </c>
+      <c r="B183" t="s">
+        <v>181</v>
+      </c>
+      <c r="C183" t="s">
+        <v>56</v>
+      </c>
+      <c r="D183" s="8">
+        <v>3.3498875104733572</v>
+      </c>
+      <c r="E183" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A184">
+        <v>20</v>
+      </c>
+      <c r="B184" t="s">
+        <v>181</v>
+      </c>
+      <c r="C184" t="s">
+        <v>56</v>
+      </c>
+      <c r="D184" s="8">
+        <v>8.3346560134937437</v>
+      </c>
+      <c r="E184" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A185">
+        <v>20</v>
+      </c>
+      <c r="B185" t="s">
+        <v>181</v>
+      </c>
+      <c r="C185" t="s">
+        <v>56</v>
+      </c>
+      <c r="D185" s="8">
+        <v>6.3330896749643468</v>
+      </c>
+      <c r="E185" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A186">
+        <v>20</v>
+      </c>
+      <c r="B186" t="s">
+        <v>181</v>
+      </c>
+      <c r="C186" t="s">
+        <v>56</v>
+      </c>
+      <c r="D186" s="8">
+        <v>0.82715430662305678</v>
+      </c>
+      <c r="E186" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A187">
+        <v>20</v>
+      </c>
+      <c r="B187" t="s">
+        <v>181</v>
+      </c>
+      <c r="C187" t="s">
+        <v>56</v>
+      </c>
+      <c r="D187" s="8">
+        <v>12.334761785472088</v>
+      </c>
+      <c r="E187" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A188">
+        <v>20</v>
+      </c>
+      <c r="B188" t="s">
+        <v>181</v>
+      </c>
+      <c r="C188" t="s">
+        <v>162</v>
+      </c>
+      <c r="D188" s="8">
+        <v>0.62926575287712383</v>
+      </c>
+      <c r="E188" t="b">
+        <v>0</v>
+      </c>
+      <c r="I188" s="8"/>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A189">
+        <v>20</v>
+      </c>
+      <c r="B189" t="s">
+        <v>180</v>
+      </c>
+      <c r="C189" t="s">
+        <v>162</v>
+      </c>
+      <c r="D189" s="8">
+        <v>1.4813329696016226</v>
+      </c>
+      <c r="E189" t="b">
+        <v>0</v>
+      </c>
+      <c r="I189" s="8"/>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A190">
+        <v>20</v>
+      </c>
+      <c r="B190" t="s">
+        <v>179</v>
+      </c>
+      <c r="C190" t="s">
+        <v>162</v>
+      </c>
+      <c r="D190" s="8">
+        <v>1</v>
+      </c>
+      <c r="E190" t="b">
+        <v>0</v>
+      </c>
+      <c r="I190" s="8"/>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A191">
+        <v>20</v>
+      </c>
+      <c r="B191" t="s">
+        <v>181</v>
+      </c>
+      <c r="C191" t="s">
+        <v>162</v>
+      </c>
+      <c r="D191" s="8">
+        <v>8.4712330715386397</v>
+      </c>
+      <c r="E191" t="b">
+        <v>0</v>
+      </c>
+      <c r="I191" s="8"/>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A192">
+        <v>20</v>
+      </c>
+      <c r="B192" t="s">
+        <v>180</v>
+      </c>
+      <c r="C192" t="s">
+        <v>162</v>
+      </c>
+      <c r="D192" s="8">
+        <v>2.193379100598857</v>
+      </c>
+      <c r="E192" t="b">
+        <v>0</v>
+      </c>
+      <c r="I192" s="8"/>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A193">
+        <v>20</v>
+      </c>
+      <c r="B193" t="s">
+        <v>179</v>
+      </c>
+      <c r="C193" t="s">
+        <v>162</v>
+      </c>
+      <c r="D193" s="8">
+        <v>1</v>
+      </c>
+      <c r="E193" t="b">
+        <v>0</v>
+      </c>
+      <c r="I193" s="8"/>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A194">
+        <v>20</v>
+      </c>
+      <c r="B194" t="s">
+        <v>181</v>
+      </c>
+      <c r="C194" t="s">
+        <v>162</v>
+      </c>
+      <c r="D194" s="8">
+        <v>7.2401684522156904</v>
+      </c>
+      <c r="E194" t="b">
+        <v>0</v>
+      </c>
+      <c r="I194" s="8"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A195">
+        <v>20</v>
+      </c>
+      <c r="B195" t="s">
+        <v>180</v>
+      </c>
+      <c r="C195" t="s">
+        <v>162</v>
+      </c>
+      <c r="D195" s="8">
+        <v>2.8798616356860864</v>
+      </c>
+      <c r="E195" t="b">
+        <v>0</v>
+      </c>
+      <c r="I195" s="8"/>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A196">
+        <v>20</v>
+      </c>
+      <c r="B196" t="s">
+        <v>179</v>
+      </c>
+      <c r="C196" t="s">
+        <v>162</v>
+      </c>
+      <c r="D196" s="8">
+        <v>1</v>
+      </c>
+      <c r="E196" t="b">
+        <v>0</v>
+      </c>
+      <c r="I196" s="8"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A197">
+        <v>20</v>
+      </c>
+      <c r="B197" t="s">
+        <v>181</v>
+      </c>
+      <c r="C197" t="s">
+        <v>162</v>
+      </c>
+      <c r="D197" s="8">
+        <v>4.9186883858404551</v>
+      </c>
+      <c r="E197" t="b">
+        <v>0</v>
+      </c>
+      <c r="I197" s="8"/>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A198">
+        <v>20</v>
+      </c>
+      <c r="B198" t="s">
+        <v>180</v>
+      </c>
+      <c r="C198" t="s">
+        <v>162</v>
+      </c>
+      <c r="D198" s="8">
+        <v>2.4557101522683311</v>
+      </c>
+      <c r="E198" t="b">
+        <v>0</v>
+      </c>
+      <c r="I198" s="8"/>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A199">
+        <v>20</v>
+      </c>
+      <c r="B199" t="s">
+        <v>179</v>
+      </c>
+      <c r="C199" t="s">
+        <v>162</v>
+      </c>
+      <c r="D199" s="8">
+        <v>1</v>
+      </c>
+      <c r="E199" t="b">
+        <v>0</v>
+      </c>
+      <c r="I199" s="8"/>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A200">
+        <v>20</v>
+      </c>
+      <c r="B200" t="s">
+        <v>181</v>
+      </c>
+      <c r="C200" t="s">
+        <v>162</v>
+      </c>
+      <c r="D200" s="8">
+        <v>6.6619319408771291</v>
+      </c>
+      <c r="E200" t="b">
+        <v>0</v>
+      </c>
+      <c r="I200" s="8"/>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A201">
+        <v>20</v>
+      </c>
+      <c r="B201" t="s">
+        <v>180</v>
+      </c>
+      <c r="C201" t="s">
+        <v>162</v>
+      </c>
+      <c r="D201" s="8">
+        <v>1.1542815525474373</v>
+      </c>
+      <c r="E201" t="b">
+        <v>0</v>
+      </c>
+      <c r="I201" s="8"/>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A202">
+        <v>20</v>
+      </c>
+      <c r="B202" t="s">
+        <v>179</v>
+      </c>
+      <c r="C202" t="s">
+        <v>162</v>
+      </c>
+      <c r="D202" s="8">
+        <v>1</v>
+      </c>
+      <c r="E202" t="b">
+        <v>0</v>
+      </c>
+      <c r="I202" s="8"/>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A203">
+        <v>20</v>
+      </c>
+      <c r="B203" t="s">
+        <v>181</v>
+      </c>
+      <c r="C203" t="s">
+        <v>162</v>
+      </c>
+      <c r="D203" s="8">
+        <v>1.549177517412722</v>
+      </c>
+      <c r="E203" t="b">
+        <v>0</v>
+      </c>
+      <c r="I203" s="8"/>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A204">
+        <v>20</v>
+      </c>
+      <c r="B204" t="s">
+        <v>180</v>
+      </c>
+      <c r="C204" t="s">
+        <v>162</v>
+      </c>
+      <c r="D204" s="8">
+        <v>1.1568740304497094</v>
+      </c>
+      <c r="E204" t="b">
+        <v>0</v>
+      </c>
+      <c r="I204" s="8"/>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A205">
+        <v>20</v>
+      </c>
+      <c r="B205" t="s">
+        <v>179</v>
+      </c>
+      <c r="C205" t="s">
+        <v>162</v>
+      </c>
+      <c r="D205" s="8">
+        <v>1</v>
+      </c>
+      <c r="E205" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A206">
+        <v>20</v>
+      </c>
+      <c r="B206" t="s">
+        <v>180</v>
+      </c>
+      <c r="C206" t="s">
+        <v>56</v>
+      </c>
+      <c r="D206" s="8">
+        <v>1.0067513807074795</v>
+      </c>
+      <c r="E206" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A207">
+        <v>20</v>
+      </c>
+      <c r="B207" t="s">
+        <v>180</v>
+      </c>
+      <c r="C207" t="s">
+        <v>56</v>
+      </c>
+      <c r="D207" s="8">
+        <v>1.3860580087485403</v>
+      </c>
+      <c r="E207" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A208">
+        <v>20</v>
+      </c>
+      <c r="B208" t="s">
+        <v>180</v>
+      </c>
+      <c r="C208" t="s">
+        <v>56</v>
+      </c>
+      <c r="D208" s="8">
+        <v>2.6895728770310723</v>
+      </c>
+      <c r="E208" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A209">
+        <v>20</v>
+      </c>
+      <c r="B209" t="s">
+        <v>180</v>
+      </c>
+      <c r="C209" t="s">
+        <v>56</v>
+      </c>
+      <c r="D209" s="8">
+        <v>2.3511568400627958</v>
+      </c>
+      <c r="E209" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A210">
+        <v>20</v>
+      </c>
+      <c r="B210" t="s">
+        <v>180</v>
+      </c>
+      <c r="C210" t="s">
+        <v>56</v>
+      </c>
+      <c r="D210" s="8">
+        <v>0.50608861879188216</v>
+      </c>
+      <c r="E210" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A211">
+        <v>20</v>
+      </c>
+      <c r="B211" t="s">
+        <v>180</v>
+      </c>
+      <c r="C211" t="s">
+        <v>56</v>
+      </c>
+      <c r="D211" s="8">
+        <v>1.2252027301372606</v>
+      </c>
+      <c r="E211" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A212">
+        <v>20</v>
+      </c>
+      <c r="B212" t="s">
+        <v>179</v>
+      </c>
+      <c r="C212" t="s">
+        <v>56</v>
+      </c>
+      <c r="D212" s="8">
+        <v>1</v>
+      </c>
+      <c r="E212" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A213">
+        <v>20</v>
+      </c>
+      <c r="B213" t="s">
+        <v>179</v>
+      </c>
+      <c r="C213" t="s">
+        <v>56</v>
+      </c>
+      <c r="D213" s="8">
+        <v>1</v>
+      </c>
+      <c r="E213" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A214">
+        <v>20</v>
+      </c>
+      <c r="B214" t="s">
+        <v>179</v>
+      </c>
+      <c r="C214" t="s">
+        <v>56</v>
+      </c>
+      <c r="D214" s="8">
+        <v>1</v>
+      </c>
+      <c r="E214" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A215">
+        <v>20</v>
+      </c>
+      <c r="B215" t="s">
+        <v>179</v>
+      </c>
+      <c r="C215" t="s">
+        <v>56</v>
+      </c>
+      <c r="D215" s="8">
+        <v>1</v>
+      </c>
+      <c r="E215" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A216">
+        <v>20</v>
+      </c>
+      <c r="B216" t="s">
+        <v>179</v>
+      </c>
+      <c r="C216" t="s">
+        <v>56</v>
+      </c>
+      <c r="D216" s="8">
+        <v>1</v>
+      </c>
+      <c r="E216" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A217">
+        <v>20</v>
+      </c>
+      <c r="B217" t="s">
+        <v>179</v>
+      </c>
+      <c r="C217" t="s">
+        <v>56</v>
+      </c>
+      <c r="D217" s="8">
+        <v>1</v>
+      </c>
+      <c r="E217" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:B205" xr:uid="{728D1403-E502-4946-B7CC-5E0361800552}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5AAFFED5B596D4BAE4CE19A95039785" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb12f4776e238e1f586e33791f07bb77">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d40adf4f-7ef1-43d3-876d-177d4150ba93" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fdb1f1d4a4ea75ce4d5cd3fd2a25377c" ns3:_="">
     <xsd:import namespace="d40adf4f-7ef1-43d3-876d-177d4150ba93"/>
@@ -15100,35 +18866,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29811117-64F0-425E-BDF0-8D1838742348}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34B288BE-7AE7-404E-A200-18C81F874FA2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d40adf4f-7ef1-43d3-876d-177d4150ba93"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15150,9 +18891,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34B288BE-7AE7-404E-A200-18C81F874FA2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29811117-64F0-425E-BDF0-8D1838742348}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d40adf4f-7ef1-43d3-876d-177d4150ba93"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updates following Ann's comments to paper draft 1 11/28/20
</commit_message>
<xml_diff>
--- a/Gene_temp_data.xlsx
+++ b/Gene_temp_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linzm\Documents\Tate_Lab_Rotation\Tate_Rotation_Temp_Immunity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EF5291-51AF-4196-AEC8-F9835E720318}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA235E0E-8E56-478B-8A46-21A7632EB1A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" tabRatio="679" firstSheet="2" activeTab="8" xr2:uid="{B3C2EB18-1E1E-4520-B7BE-6EC39DD43585}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2371" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2371" uniqueCount="201">
   <si>
     <t>Well Position</t>
   </si>
@@ -671,6 +671,12 @@
   </si>
   <si>
     <t>Rate</t>
+  </si>
+  <si>
+    <t>Microbe_Independent_Rate</t>
+  </si>
+  <si>
+    <t>Microbe_Dependent_Rate</t>
   </si>
 </sst>
 </file>
@@ -3051,7 +3057,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="13447713" y="166688"/>
+              <a:off x="19962813" y="166688"/>
               <a:ext cx="5769767" cy="4486274"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -21389,7 +21395,7 @@
   <dimension ref="A1:E145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -21419,7 +21425,7 @@
         <v>190</v>
       </c>
       <c r="C2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D2">
         <v>0.73160000000000003</v>
@@ -21436,7 +21442,7 @@
         <v>190</v>
       </c>
       <c r="C3" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D3">
         <v>0.76327499999999993</v>
@@ -21453,7 +21459,7 @@
         <v>190</v>
       </c>
       <c r="C4" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D4">
         <v>0.33252500000000002</v>
@@ -21470,7 +21476,7 @@
         <v>190</v>
       </c>
       <c r="C5" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D5">
         <v>3.04765</v>
@@ -21487,7 +21493,7 @@
         <v>190</v>
       </c>
       <c r="C6" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D6" t="e">
         <v>#VALUE!</v>
@@ -21504,7 +21510,7 @@
         <v>190</v>
       </c>
       <c r="C7" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D7" t="e">
         <v>#VALUE!</v>
@@ -21521,7 +21527,7 @@
         <v>190</v>
       </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D8">
         <v>0.40900000000000003</v>
@@ -21538,7 +21544,7 @@
         <v>190</v>
       </c>
       <c r="C9" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D9">
         <v>0.95307499999999989</v>
@@ -21555,7 +21561,7 @@
         <v>190</v>
       </c>
       <c r="C10" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D10">
         <v>1.9866249999999999</v>
@@ -21572,7 +21578,7 @@
         <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D11">
         <v>0.519675</v>
@@ -21589,7 +21595,7 @@
         <v>190</v>
       </c>
       <c r="C12" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D12" t="e">
         <v>#VALUE!</v>
@@ -21606,7 +21612,7 @@
         <v>190</v>
       </c>
       <c r="C13" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D13" t="e">
         <v>#VALUE!</v>
@@ -21623,7 +21629,7 @@
         <v>190</v>
       </c>
       <c r="C14" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D14">
         <v>-0.13922499999999999</v>
@@ -21640,7 +21646,7 @@
         <v>190</v>
       </c>
       <c r="C15" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D15">
         <v>0.23992500000000005</v>
@@ -21657,7 +21663,7 @@
         <v>190</v>
       </c>
       <c r="C16" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D16">
         <v>0.38127500000000003</v>
@@ -21674,7 +21680,7 @@
         <v>190</v>
       </c>
       <c r="C17" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D17">
         <v>-6.2775000000000025E-2</v>
@@ -21691,7 +21697,7 @@
         <v>190</v>
       </c>
       <c r="C18" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D18" t="e">
         <v>#VALUE!</v>
@@ -21708,7 +21714,7 @@
         <v>190</v>
       </c>
       <c r="C19" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D19" t="e">
         <v>#VALUE!</v>
@@ -21725,7 +21731,7 @@
         <v>190</v>
       </c>
       <c r="C20" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D20">
         <v>0.40900000000000003</v>
@@ -21742,7 +21748,7 @@
         <v>190</v>
       </c>
       <c r="C21" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D21">
         <v>0.95307499999999989</v>
@@ -21759,7 +21765,7 @@
         <v>190</v>
       </c>
       <c r="C22" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D22">
         <v>1.9866249999999999</v>
@@ -21776,7 +21782,7 @@
         <v>190</v>
       </c>
       <c r="C23" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D23">
         <v>0.519675</v>
@@ -21793,7 +21799,7 @@
         <v>190</v>
       </c>
       <c r="C24" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D24" t="e">
         <v>#VALUE!</v>
@@ -21810,7 +21816,7 @@
         <v>190</v>
       </c>
       <c r="C25" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D25" t="e">
         <v>#VALUE!</v>
@@ -21827,7 +21833,7 @@
         <v>190</v>
       </c>
       <c r="C26" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D26">
         <v>12.553775000000002</v>
@@ -21844,7 +21850,7 @@
         <v>190</v>
       </c>
       <c r="C27" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D27">
         <v>4.8487</v>
@@ -21861,7 +21867,7 @@
         <v>190</v>
       </c>
       <c r="C28" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D28">
         <v>10.886150000000001</v>
@@ -21878,7 +21884,7 @@
         <v>190</v>
       </c>
       <c r="C29" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D29">
         <v>7.8204500000000001</v>
@@ -21895,7 +21901,7 @@
         <v>190</v>
       </c>
       <c r="C30" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D30" t="e">
         <v>#VALUE!</v>
@@ -21912,7 +21918,7 @@
         <v>190</v>
       </c>
       <c r="C31" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D31" t="e">
         <v>#VALUE!</v>
@@ -21929,7 +21935,7 @@
         <v>190</v>
       </c>
       <c r="C32" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D32">
         <v>2.6326749999999999</v>
@@ -21946,7 +21952,7 @@
         <v>190</v>
       </c>
       <c r="C33" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D33">
         <v>1.8601750000000001</v>
@@ -21963,7 +21969,7 @@
         <v>190</v>
       </c>
       <c r="C34" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D34">
         <v>2.8611999999999997</v>
@@ -21980,7 +21986,7 @@
         <v>190</v>
       </c>
       <c r="C35" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D35">
         <v>1.3976</v>
@@ -21997,7 +22003,7 @@
         <v>190</v>
       </c>
       <c r="C36" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D36">
         <v>6.2445750000000002</v>
@@ -22014,7 +22020,7 @@
         <v>190</v>
       </c>
       <c r="C37" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D37">
         <v>-9.4299999999999995E-2</v>
@@ -22031,7 +22037,7 @@
         <v>190</v>
       </c>
       <c r="C38" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D38">
         <v>5.21265</v>
@@ -22048,7 +22054,7 @@
         <v>190</v>
       </c>
       <c r="C39" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D39">
         <v>2.5057750000000003</v>
@@ -22065,7 +22071,7 @@
         <v>190</v>
       </c>
       <c r="C40" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D40">
         <v>2.4590749999999999</v>
@@ -22082,7 +22088,7 @@
         <v>190</v>
       </c>
       <c r="C41" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D41">
         <v>0.96</v>
@@ -22099,7 +22105,7 @@
         <v>190</v>
       </c>
       <c r="C42" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D42" t="e">
         <v>#VALUE!</v>
@@ -22116,7 +22122,7 @@
         <v>190</v>
       </c>
       <c r="C43" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D43">
         <v>0.23477500000000001</v>
@@ -22133,7 +22139,7 @@
         <v>190</v>
       </c>
       <c r="C44" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D44">
         <v>2.6326749999999999</v>
@@ -22150,7 +22156,7 @@
         <v>190</v>
       </c>
       <c r="C45" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D45">
         <v>1.8601750000000001</v>
@@ -22167,7 +22173,7 @@
         <v>190</v>
       </c>
       <c r="C46" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D46">
         <v>2.8611999999999997</v>
@@ -22184,7 +22190,7 @@
         <v>190</v>
       </c>
       <c r="C47" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D47">
         <v>1.3976</v>
@@ -22201,7 +22207,7 @@
         <v>190</v>
       </c>
       <c r="C48" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D48">
         <v>6.2445750000000002</v>
@@ -22218,7 +22224,7 @@
         <v>190</v>
       </c>
       <c r="C49" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D49">
         <v>-9.4299999999999995E-2</v>
@@ -22235,7 +22241,7 @@
         <v>56</v>
       </c>
       <c r="C50" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D50">
         <v>1.8640258186287457</v>
@@ -22252,7 +22258,7 @@
         <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D51">
         <v>3.3410274787169825</v>
@@ -22269,7 +22275,7 @@
         <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D52">
         <v>5.5736897481267293</v>
@@ -22286,7 +22292,7 @@
         <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D53">
         <v>3.0641520943480396</v>
@@ -22303,7 +22309,7 @@
         <v>56</v>
       </c>
       <c r="C54" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D54">
         <v>3.2279892998511244</v>
@@ -22320,7 +22326,7 @@
         <v>56</v>
       </c>
       <c r="C55" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D55">
         <v>3.094545363816307</v>
@@ -22337,7 +22343,7 @@
         <v>56</v>
       </c>
       <c r="C56" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D56">
         <v>0.27617708270881625</v>
@@ -22354,7 +22360,7 @@
         <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D57">
         <v>0.5874718776183393</v>
@@ -22371,7 +22377,7 @@
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D58">
         <v>1.8336640033734359</v>
@@ -22388,7 +22394,7 @@
         <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D59">
         <v>1.3332724187410867</v>
@@ -22405,7 +22411,7 @@
         <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D60">
         <v>-4.3211423344235805E-2</v>
@@ -22422,7 +22428,7 @@
         <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D61">
         <v>2.8336904463680219</v>
@@ -22439,7 +22445,7 @@
         <v>56</v>
       </c>
       <c r="C62" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D62">
         <v>0.62397286337625812</v>
@@ -22456,7 +22462,7 @@
         <v>56</v>
       </c>
       <c r="C63" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D63">
         <v>0.38515323037193927</v>
@@ -22473,7 +22479,7 @@
         <v>56</v>
       </c>
       <c r="C64" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D64">
         <v>1.0404876593724939</v>
@@ -22490,7 +22496,7 @@
         <v>56</v>
       </c>
       <c r="C65" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D65">
         <v>1.1074919468402264</v>
@@ -22507,7 +22513,7 @@
         <v>56</v>
       </c>
       <c r="C66" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D66">
         <v>0.66910754108978732</v>
@@ -22524,7 +22530,7 @@
         <v>56</v>
       </c>
       <c r="C67" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D67">
         <v>2.0854358668251765</v>
@@ -22541,7 +22547,7 @@
         <v>56</v>
       </c>
       <c r="C68" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D68">
         <v>0.27617708270881625</v>
@@ -22558,7 +22564,7 @@
         <v>56</v>
       </c>
       <c r="C69" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D69">
         <v>0.5874718776183393</v>
@@ -22575,7 +22581,7 @@
         <v>56</v>
       </c>
       <c r="C70" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D70">
         <v>1.8336640033734359</v>
@@ -22592,7 +22598,7 @@
         <v>56</v>
       </c>
       <c r="C71" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D71">
         <v>1.3332724187410867</v>
@@ -22609,7 +22615,7 @@
         <v>56</v>
       </c>
       <c r="C72" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D72">
         <v>-4.3211423344235805E-2</v>
@@ -22626,7 +22632,7 @@
         <v>56</v>
       </c>
       <c r="C73" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D73">
         <v>2.8336904463680219</v>
@@ -22643,7 +22649,7 @@
         <v>56</v>
       </c>
       <c r="C74" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D74">
         <v>0.1308946199804398</v>
@@ -22660,7 +22666,7 @@
         <v>56</v>
       </c>
       <c r="C75" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D75">
         <v>8.9000015270398913E-2</v>
@@ -22677,7 +22683,7 @@
         <v>56</v>
       </c>
       <c r="C76" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D76">
         <v>0.39288990433664694</v>
@@ -22694,7 +22700,7 @@
         <v>56</v>
       </c>
       <c r="C77" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D77">
         <v>-0.28115298985122994</v>
@@ -22711,7 +22717,7 @@
         <v>56</v>
       </c>
       <c r="C78" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D78">
         <v>0.77355901215999789</v>
@@ -22728,7 +22734,7 @@
         <v>56</v>
       </c>
       <c r="C79" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D79">
         <v>-0.46867158411392662</v>
@@ -22745,7 +22751,7 @@
         <v>56</v>
       </c>
       <c r="C80" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D80">
         <v>-2.4268627166748047E-3</v>
@@ -22762,7 +22768,7 @@
         <v>56</v>
       </c>
       <c r="C81" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D81">
         <v>9.6514502187135087E-2</v>
@@ -22779,7 +22785,7 @@
         <v>56</v>
       </c>
       <c r="C82" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D82">
         <v>0.42239321925776807</v>
@@ -22796,7 +22802,7 @@
         <v>56</v>
       </c>
       <c r="C83" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D83">
         <v>0.33778921001569895</v>
@@ -22813,7 +22819,7 @@
         <v>56</v>
       </c>
       <c r="C84" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D84">
         <v>-0.12347784530202946</v>
@@ -22830,7 +22836,7 @@
         <v>56</v>
       </c>
       <c r="C85" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D85">
         <v>5.6300682534315138E-2</v>
@@ -22847,7 +22853,7 @@
         <v>56</v>
       </c>
       <c r="C86" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D86">
         <v>-6.5687266410192846E-2</v>
@@ -22864,7 +22870,7 @@
         <v>56</v>
       </c>
       <c r="C87" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D87">
         <v>2.3930440216597071E-2</v>
@@ -22881,7 +22887,7 @@
         <v>56</v>
       </c>
       <c r="C88" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D88">
         <v>-2.5817693661473184E-2</v>
@@ -22898,7 +22904,7 @@
         <v>56</v>
       </c>
       <c r="C89" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D89">
         <v>0.32535967828076384</v>
@@ -22915,7 +22921,7 @@
         <v>56</v>
       </c>
       <c r="C90" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D90">
         <v>-2.8492832478848235E-2</v>
@@ -22932,7 +22938,7 @@
         <v>56</v>
       </c>
       <c r="C91" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D91">
         <v>5.723876400888539E-2</v>
@@ -22949,7 +22955,7 @@
         <v>56</v>
       </c>
       <c r="C92" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D92">
         <v>-2.4268627166748047E-3</v>
@@ -22966,7 +22972,7 @@
         <v>56</v>
       </c>
       <c r="C93" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D93">
         <v>9.6514502187135087E-2</v>
@@ -22983,7 +22989,7 @@
         <v>56</v>
       </c>
       <c r="C94" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D94">
         <v>0.42239321925776807</v>
@@ -23000,7 +23006,7 @@
         <v>56</v>
       </c>
       <c r="C95" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D95">
         <v>0.33778921001569895</v>
@@ -23017,7 +23023,7 @@
         <v>56</v>
       </c>
       <c r="C96" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D96">
         <v>-0.12347784530202946</v>
@@ -23034,7 +23040,7 @@
         <v>56</v>
       </c>
       <c r="C97" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D97">
         <v>5.6300682534315138E-2</v>
@@ -23051,7 +23057,7 @@
         <v>162</v>
       </c>
       <c r="C98" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D98">
         <v>0.54185242318131566</v>
@@ -23068,7 +23074,7 @@
         <v>162</v>
       </c>
       <c r="C99" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D99">
         <v>0.72049246481633777</v>
@@ -23085,7 +23091,7 @@
         <v>162</v>
       </c>
       <c r="C100" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D100">
         <v>0.57183031919067751</v>
@@ -23102,7 +23108,7 @@
         <v>162</v>
       </c>
       <c r="C101" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D101">
         <v>0.19419396035395986</v>
@@ -23119,7 +23125,7 @@
         <v>162</v>
       </c>
       <c r="C102" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D102">
         <v>0.3622535594895262</v>
@@ -23136,7 +23142,7 @@
         <v>162</v>
       </c>
       <c r="C103" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D103">
         <v>0.83191139713880102</v>
@@ -23153,7 +23159,7 @@
         <v>162</v>
       </c>
       <c r="C104" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D104">
         <v>0.12033324240040566</v>
@@ -23170,7 +23176,7 @@
         <v>162</v>
       </c>
       <c r="C105" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D105">
         <v>0.29834477514971425</v>
@@ -23187,7 +23193,7 @@
         <v>162</v>
       </c>
       <c r="C106" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D106">
         <v>0.46996540892152161</v>
@@ -23204,7 +23210,7 @@
         <v>162</v>
       </c>
       <c r="C107" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D107">
         <v>0.36392753806708278</v>
@@ -23221,7 +23227,7 @@
         <v>162</v>
       </c>
       <c r="C108" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D108">
         <v>3.8570388136859313E-2</v>
@@ -23238,7 +23244,7 @@
         <v>162</v>
       </c>
       <c r="C109" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D109">
         <v>3.9218507612427345E-2</v>
@@ -23255,7 +23261,7 @@
         <v>162</v>
       </c>
       <c r="C110" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D110">
         <v>0.48585548760646813</v>
@@ -23272,7 +23278,7 @@
         <v>162</v>
       </c>
       <c r="C111" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D111">
         <v>0.12284130184435788</v>
@@ -23289,7 +23295,7 @@
         <v>162</v>
       </c>
       <c r="C112" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D112">
         <v>0.13163913938961397</v>
@@ -23306,7 +23312,7 @@
         <v>162</v>
       </c>
       <c r="C113" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D113">
         <v>0.38402956707166619</v>
@@ -23323,7 +23329,7 @@
         <v>162</v>
       </c>
       <c r="C114" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D114">
         <v>0.15142250139452493</v>
@@ -23340,7 +23346,7 @@
         <v>162</v>
       </c>
       <c r="C115" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D115">
         <v>-6.3165898501745796E-2</v>
@@ -23357,7 +23363,7 @@
         <v>162</v>
       </c>
       <c r="C116" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D116">
         <v>0.12033324240040566</v>
@@ -23374,7 +23380,7 @@
         <v>162</v>
       </c>
       <c r="C117" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D117">
         <v>0.29834477514971425</v>
@@ -23391,7 +23397,7 @@
         <v>162</v>
       </c>
       <c r="C118" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D118">
         <v>0.46996540892152161</v>
@@ -23408,7 +23414,7 @@
         <v>162</v>
       </c>
       <c r="C119" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D119">
         <v>0.36392753806708278</v>
@@ -23425,7 +23431,7 @@
         <v>162</v>
       </c>
       <c r="C120" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D120">
         <v>3.8570388136859313E-2</v>
@@ -23442,7 +23448,7 @@
         <v>162</v>
       </c>
       <c r="C121" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D121">
         <v>3.9218507612427345E-2</v>
@@ -23459,7 +23465,7 @@
         <v>162</v>
       </c>
       <c r="C122" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D122">
         <v>0.49325861352315237</v>
@@ -23476,7 +23482,7 @@
         <v>162</v>
       </c>
       <c r="C123" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D123">
         <v>5.8698872553787549</v>
@@ -23493,7 +23499,7 @@
         <v>162</v>
       </c>
       <c r="C124" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D124">
         <v>5.5243990709911373</v>
@@ -23510,7 +23516,7 @@
         <v>162</v>
       </c>
       <c r="C125" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D125">
         <v>2.372756097791282</v>
@@ -23527,7 +23533,7 @@
         <v>162</v>
       </c>
       <c r="C126" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D126">
         <v>-4.1071830038581392E-2</v>
@@ -23544,7 +23550,7 @@
         <v>162</v>
       </c>
       <c r="C127" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D127">
         <v>4.1991479639061673</v>
@@ -23561,7 +23567,7 @@
         <v>162</v>
       </c>
       <c r="C128" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D128">
         <v>-9.2683561780719043E-2</v>
@@ -23578,7 +23584,7 @@
         <v>162</v>
       </c>
       <c r="C129" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D129">
         <v>1.8678082678846599</v>
@@ -23595,7 +23601,7 @@
         <v>162</v>
       </c>
       <c r="C130" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D130">
         <v>1.5600421130539226</v>
@@ -23612,7 +23618,7 @@
         <v>162</v>
       </c>
       <c r="C131" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D131">
         <v>0.97967209646011377</v>
@@ -23629,7 +23635,7 @@
         <v>162</v>
       </c>
       <c r="C132" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D132">
         <v>1.4154829852192823</v>
@@ -23646,7 +23652,7 @@
         <v>162</v>
       </c>
       <c r="C133" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D133">
         <v>0.13729437935318051</v>
@@ -23663,7 +23669,7 @@
         <v>162</v>
       </c>
       <c r="C134" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D134">
         <v>5.8528871628093828</v>
@@ -23680,7 +23686,7 @@
         <v>162</v>
       </c>
       <c r="C135" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D135">
         <v>2.7219735587374072</v>
@@ -23697,7 +23703,7 @@
         <v>162</v>
       </c>
       <c r="C136" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D136">
         <v>1.6411479037231014</v>
@@ -23714,7 +23720,7 @@
         <v>162</v>
       </c>
       <c r="C137" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D137">
         <v>0.48477234769690153</v>
@@ -23731,7 +23737,7 @@
         <v>162</v>
       </c>
       <c r="C138" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D138">
         <v>0.49183115631299346</v>
@@ -23748,7 +23754,7 @@
         <v>162</v>
       </c>
       <c r="C139" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D139">
         <v>0.34585259100746923</v>
@@ -23765,7 +23771,7 @@
         <v>162</v>
       </c>
       <c r="C140" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D140">
         <v>-9.2683561780719043E-2</v>
@@ -23782,7 +23788,7 @@
         <v>162</v>
       </c>
       <c r="C141" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D141">
         <v>1.8678082678846599</v>
@@ -23799,7 +23805,7 @@
         <v>162</v>
       </c>
       <c r="C142" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D142">
         <v>1.5600421130539226</v>
@@ -23816,7 +23822,7 @@
         <v>162</v>
       </c>
       <c r="C143" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D143">
         <v>0.97967209646011377</v>
@@ -23833,7 +23839,7 @@
         <v>162</v>
       </c>
       <c r="C144" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D144">
         <v>1.4154829852192823</v>
@@ -23850,7 +23856,7 @@
         <v>162</v>
       </c>
       <c r="C145" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D145">
         <v>0.13729437935318051</v>
@@ -24029,18 +24035,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24062,6 +24068,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34B288BE-7AE7-404E-A200-18C81F874FA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6078DB98-64DD-44CA-A39B-9F3CF9F2C375}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -24075,12 +24089,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34B288BE-7AE7-404E-A200-18C81F874FA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>